<commit_message>
Update field resolution figures and tables
</commit_message>
<xml_diff>
--- a/figures+tables/Tables_FitStats_Formatted.xlsx
+++ b/figures+tables/Tables_FitStats_Formatted.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s947z036\WorkGits\SD-6_MapWaterConservation\figures+tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEC7125-535C-403A-A347-2DCC87B0F4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C965C74-7257-4432-AAA4-949D1755E81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="8880" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1 - copy raw data here" sheetId="1" r:id="rId1"/>
-    <sheet name="Table 1 formatted" sheetId="3" r:id="rId2"/>
-    <sheet name="Table S1 copy raw data" sheetId="7" r:id="rId3"/>
-    <sheet name="Table S1 Precip corrected table" sheetId="4" r:id="rId4"/>
-    <sheet name="Table 2 - copy raw data here" sheetId="10" r:id="rId5"/>
-    <sheet name="Table 2 formatted" sheetId="11" r:id="rId6"/>
-    <sheet name="Table 3 - copy raw data here" sheetId="5" r:id="rId7"/>
-    <sheet name="Table 3 formatted" sheetId="6" r:id="rId8"/>
+    <sheet name="Table 1 field - raw data" sheetId="5" r:id="rId1"/>
+    <sheet name="Table 1 field - formatted" sheetId="6" r:id="rId2"/>
+    <sheet name="Table 1 - copy raw data here" sheetId="1" r:id="rId3"/>
+    <sheet name="Table 1 formatted" sheetId="3" r:id="rId4"/>
+    <sheet name="Table S1 copy raw data" sheetId="7" r:id="rId5"/>
+    <sheet name="Table S1 Precip corrected table" sheetId="4" r:id="rId6"/>
+    <sheet name="Table 2 - copy raw data here" sheetId="10" r:id="rId7"/>
+    <sheet name="Table 2 formatted" sheetId="11" r:id="rId8"/>
     <sheet name="Table S2 - copy raw data here" sheetId="8" r:id="rId9"/>
     <sheet name="Table S2 formatted" sheetId="9" r:id="rId10"/>
   </sheets>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="68">
   <si>
     <t>Algorithm</t>
   </si>
@@ -381,6 +381,9 @@
   </si>
   <si>
     <t>Area Agree</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -635,7 +638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -877,6 +880,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -884,21 +893,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1181,345 +1175,313 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08A1325-ED28-4898-AD5B-BD59E01EE5C5}">
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>65.400000000000006</v>
+        <v>1.9</v>
       </c>
       <c r="C2">
-        <v>46.8</v>
+        <v>85.409042072712595</v>
       </c>
       <c r="D2">
-        <v>50.6</v>
+        <v>0.47934391039936097</v>
       </c>
       <c r="E2">
-        <v>1.3264925760619399</v>
-      </c>
-      <c r="F2">
-        <v>0.94977537606193996</v>
-      </c>
-      <c r="G2">
-        <v>1.1936025751473101</v>
-      </c>
-      <c r="H2">
-        <v>0.70722325678104503</v>
-      </c>
-      <c r="I2">
-        <v>0.69082503808143803</v>
-      </c>
-      <c r="J2">
-        <v>0.31761842437134202</v>
-      </c>
-      <c r="K2">
-        <v>0.40690748489495798</v>
-      </c>
-      <c r="L2">
-        <v>0.43274806461895099</v>
-      </c>
-      <c r="M2">
-        <v>0.22662206988995201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.83154654539522899</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>108.6</v>
+        <v>27.7</v>
       </c>
       <c r="C3">
-        <v>98.5</v>
+        <v>125.61152250940501</v>
       </c>
       <c r="D3">
-        <v>91.5</v>
+        <v>0.45564596176653299</v>
       </c>
       <c r="E3">
-        <v>2.2049506480619399</v>
-      </c>
-      <c r="F3">
-        <v>2.00024414806194</v>
-      </c>
-      <c r="G3">
-        <v>1.85773088406194</v>
-      </c>
-      <c r="H3">
-        <v>0.96546512071329205</v>
-      </c>
-      <c r="I3">
-        <v>0.87769876929967305</v>
-      </c>
-      <c r="J3">
-        <v>0.63712450373597496</v>
-      </c>
-      <c r="K3">
-        <v>0.377574803193928</v>
-      </c>
-      <c r="L3">
-        <v>0.38775196783792598</v>
-      </c>
-      <c r="M3">
-        <v>0.28503364673370002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.59482236220801998</v>
+      </c>
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4">
-        <v>75</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C4">
-        <v>67.5</v>
+        <v>80.742612914364599</v>
       </c>
       <c r="D4">
-        <v>60.2</v>
+        <v>0.53439781105966999</v>
       </c>
       <c r="E4">
-        <v>1.5220841060619399</v>
-      </c>
-      <c r="F4">
-        <v>1.3702253440619401</v>
-      </c>
-      <c r="G4">
-        <v>1.2227832780619401</v>
-      </c>
-      <c r="H4">
-        <v>0.98047507399070599</v>
-      </c>
-      <c r="I4">
-        <v>0.93019406011203898</v>
-      </c>
-      <c r="J4">
-        <v>0.67053346789159896</v>
-      </c>
-      <c r="K4">
-        <v>0.41951285242667402</v>
-      </c>
-      <c r="L4">
-        <v>0.46811426299519598</v>
-      </c>
-      <c r="M4">
-        <v>0.33694581169332799</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.88172670086260097</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5">
-        <v>30.1</v>
+        <v>-34</v>
       </c>
       <c r="C5">
-        <v>25.4</v>
+        <v>136.469390294703</v>
       </c>
       <c r="D5">
-        <v>18.8</v>
+        <v>0.45918218601229299</v>
       </c>
       <c r="E5">
-        <v>0.83586382093317102</v>
-      </c>
-      <c r="F5">
-        <v>0.60332796572881597</v>
-      </c>
-      <c r="G5">
-        <v>0.88872024081419099</v>
-      </c>
-      <c r="H5">
-        <v>0.95987013370315999</v>
-      </c>
-      <c r="I5">
-        <v>0.88673729685160996</v>
-      </c>
-      <c r="J5">
-        <v>0.71027998243946699</v>
-      </c>
-      <c r="K5">
-        <v>0.35680908719869198</v>
-      </c>
-      <c r="L5">
-        <v>0.39691877484075699</v>
-      </c>
-      <c r="M5">
-        <v>0.30625140776853899</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.78867260709596898</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6">
-        <v>63</v>
+        <v>-11.9</v>
       </c>
       <c r="C6">
-        <v>54.8</v>
+        <v>95.162962508470898</v>
       </c>
       <c r="D6">
-        <v>49.4</v>
+        <v>0.41071267036243903</v>
       </c>
       <c r="E6">
-        <v>1.2791523360619399</v>
-      </c>
-      <c r="F6">
-        <v>1.11282718006194</v>
-      </c>
-      <c r="G6">
-        <v>1.0036873200619401</v>
-      </c>
-      <c r="H6">
-        <v>0.97827409490972295</v>
-      </c>
-      <c r="I6">
-        <v>0.91565097784484495</v>
-      </c>
-      <c r="J6">
-        <v>0.64345323564458301</v>
-      </c>
-      <c r="K6">
-        <v>0.417700106510139</v>
-      </c>
-      <c r="L6">
-        <v>0.46456133905040398</v>
-      </c>
-      <c r="M6">
-        <v>0.32831283047439103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.956205473395907</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7">
-        <v>165.6</v>
+        <v>47.5</v>
       </c>
       <c r="C7">
-        <v>144.4</v>
+        <v>182.213076546927</v>
       </c>
       <c r="D7">
-        <v>149.9</v>
+        <v>0.37127104234382302</v>
       </c>
       <c r="E7">
-        <v>3.3609131600619402</v>
-      </c>
-      <c r="F7">
-        <v>2.9305214960619401</v>
-      </c>
-      <c r="G7">
-        <v>3.0432672320619401</v>
-      </c>
-      <c r="H7">
-        <v>0.98400599280103296</v>
-      </c>
-      <c r="I7">
-        <v>0.93078577029168597</v>
-      </c>
-      <c r="J7">
-        <v>0.568102088811406</v>
-      </c>
-      <c r="K7">
-        <v>0.54931383902197095</v>
-      </c>
-      <c r="L7">
-        <v>0.60926055216130204</v>
-      </c>
-      <c r="M7">
-        <v>0.42013696880208601</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.81353933321874194</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8">
-        <v>48.7</v>
+        <v>10.8</v>
       </c>
       <c r="C8">
-        <v>60.5</v>
+        <v>96.040602314077503</v>
       </c>
       <c r="D8">
-        <v>33.9</v>
+        <v>0.47145600078347299</v>
       </c>
       <c r="E8">
-        <v>0.98815472206193999</v>
-      </c>
-      <c r="F8">
-        <v>1.2283358760619401</v>
-      </c>
-      <c r="G8">
-        <v>0.86337590372881601</v>
-      </c>
-      <c r="H8">
-        <v>0.96972039389537301</v>
-      </c>
-      <c r="I8">
-        <v>0.90988591409012798</v>
-      </c>
-      <c r="J8">
-        <v>0.69401816999657095</v>
-      </c>
-      <c r="K8">
-        <v>0.441917209407449</v>
-      </c>
-      <c r="L8">
-        <v>0.48907248286788402</v>
-      </c>
-      <c r="M8">
-        <v>0.37111742539425402</v>
+        <v>0.65032885421767295</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>-1.5</v>
+      </c>
+      <c r="C9">
+        <v>51.906975818498097</v>
+      </c>
+      <c r="D9">
+        <v>0.70532777929520796</v>
+      </c>
+      <c r="E9">
+        <v>1.1840507942490699</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>22.7</v>
+      </c>
+      <c r="C10">
+        <v>93.020879625713803</v>
+      </c>
+      <c r="D10">
+        <v>0.66363739375391695</v>
+      </c>
+      <c r="E10">
+        <v>0.87784853814363795</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>1.6</v>
+      </c>
+      <c r="C11">
+        <v>48.493179228569602</v>
+      </c>
+      <c r="D11">
+        <v>0.741080973339585</v>
+      </c>
+      <c r="E11">
+        <v>1.21516453360651</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>-35.200000000000003</v>
+      </c>
+      <c r="C12">
+        <v>125.702055063413</v>
+      </c>
+      <c r="D12">
+        <v>0.72538247390556498</v>
+      </c>
+      <c r="E12">
+        <v>1.3100706798388</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>-13.3</v>
+      </c>
+      <c r="C13">
+        <v>69.488025912483195</v>
+      </c>
+      <c r="D13">
+        <v>0.59867515216147105</v>
+      </c>
+      <c r="E13">
+        <v>1.3824169820843699</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>41.8</v>
+      </c>
+      <c r="C14">
+        <v>158.13699958153001</v>
+      </c>
+      <c r="D14">
+        <v>0.46760521039555097</v>
+      </c>
+      <c r="E14">
+        <v>0.98572691346165997</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>6.5</v>
+      </c>
+      <c r="C15">
+        <v>51.885675813081001</v>
+      </c>
+      <c r="D15">
+        <v>0.75673728770078996</v>
+      </c>
+      <c r="E15">
+        <v>1.03324963192462</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1543,22 +1505,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="92" t="s">
+      <c r="C1" s="95"/>
+      <c r="D1" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="92" t="s">
+      <c r="E1" s="95"/>
+      <c r="F1" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="93"/>
-      <c r="H1" s="92" t="s">
+      <c r="G1" s="95"/>
+      <c r="H1" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="93"/>
+      <c r="I1" s="95"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -1897,6 +1859,722 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC122BAA-6B80-44F9-A1DF-409EA6AE6532}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="90"/>
+      <c r="B1" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="95"/>
+      <c r="D1" s="94" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="95"/>
+      <c r="F1" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="95"/>
+      <c r="H1" s="94" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="95"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="12">
+        <f>'Table 1 field - raw data'!C2</f>
+        <v>85.409042072712595</v>
+      </c>
+      <c r="C3" s="13">
+        <f>'Table 1 field - raw data'!C9</f>
+        <v>51.906975818498097</v>
+      </c>
+      <c r="D3" s="14">
+        <f>'Table 1 field - raw data'!B2</f>
+        <v>1.9</v>
+      </c>
+      <c r="E3" s="15">
+        <f>'Table 1 field - raw data'!B9</f>
+        <v>-1.5</v>
+      </c>
+      <c r="F3" s="16">
+        <f>'Table 1 field - raw data'!E2</f>
+        <v>0.83154654539522899</v>
+      </c>
+      <c r="G3" s="17">
+        <f>'Table 1 field - raw data'!E9</f>
+        <v>1.1840507942490699</v>
+      </c>
+      <c r="H3" s="16">
+        <f>'Table 1 field - raw data'!D2</f>
+        <v>0.47934391039936097</v>
+      </c>
+      <c r="I3" s="17">
+        <f>'Table 1 field - raw data'!D9</f>
+        <v>0.70532777929520796</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="19">
+        <f>'Table 1 field - raw data'!C3</f>
+        <v>125.61152250940501</v>
+      </c>
+      <c r="C4" s="20">
+        <f>'Table 1 field - raw data'!C10</f>
+        <v>93.020879625713803</v>
+      </c>
+      <c r="D4" s="21">
+        <f>'Table 1 field - raw data'!B3</f>
+        <v>27.7</v>
+      </c>
+      <c r="E4" s="22">
+        <f>'Table 1 field - raw data'!B10</f>
+        <v>22.7</v>
+      </c>
+      <c r="F4" s="23">
+        <f>'Table 1 field - raw data'!E3</f>
+        <v>0.59482236220801998</v>
+      </c>
+      <c r="G4" s="24">
+        <f>'Table 1 field - raw data'!E10</f>
+        <v>0.87784853814363795</v>
+      </c>
+      <c r="H4" s="23">
+        <f>'Table 1 field - raw data'!D3</f>
+        <v>0.45564596176653299</v>
+      </c>
+      <c r="I4" s="24">
+        <f>'Table 1 field - raw data'!D10</f>
+        <v>0.66363739375391695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="12">
+        <f>'Table 1 field - raw data'!C4</f>
+        <v>80.742612914364599</v>
+      </c>
+      <c r="C5" s="13">
+        <f>'Table 1 field - raw data'!C11</f>
+        <v>48.493179228569602</v>
+      </c>
+      <c r="D5" s="14">
+        <f>'Table 1 field - raw data'!B4</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E5" s="15">
+        <f>'Table 1 field - raw data'!B11</f>
+        <v>1.6</v>
+      </c>
+      <c r="F5" s="16">
+        <f>'Table 1 field - raw data'!E4</f>
+        <v>0.88172670086260097</v>
+      </c>
+      <c r="G5" s="17">
+        <f>'Table 1 field - raw data'!E11</f>
+        <v>1.21516453360651</v>
+      </c>
+      <c r="H5" s="16">
+        <f>'Table 1 field - raw data'!D4</f>
+        <v>0.53439781105966999</v>
+      </c>
+      <c r="I5" s="17">
+        <f>'Table 1 field - raw data'!D11</f>
+        <v>0.741080973339585</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="19">
+        <f>'Table 1 field - raw data'!C5</f>
+        <v>136.469390294703</v>
+      </c>
+      <c r="C6" s="20">
+        <f>'Table 1 field - raw data'!C12</f>
+        <v>125.702055063413</v>
+      </c>
+      <c r="D6" s="21">
+        <f>'Table 1 field - raw data'!B5</f>
+        <v>-34</v>
+      </c>
+      <c r="E6" s="22">
+        <f>'Table 1 field - raw data'!B12</f>
+        <v>-35.200000000000003</v>
+      </c>
+      <c r="F6" s="23">
+        <f>'Table 1 field - raw data'!E5</f>
+        <v>0.78867260709596898</v>
+      </c>
+      <c r="G6" s="24">
+        <f>'Table 1 field - raw data'!E12</f>
+        <v>1.3100706798388</v>
+      </c>
+      <c r="H6" s="23">
+        <f>'Table 1 field - raw data'!D5</f>
+        <v>0.45918218601229299</v>
+      </c>
+      <c r="I6" s="24">
+        <f>'Table 1 field - raw data'!D12</f>
+        <v>0.72538247390556498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="12">
+        <f>'Table 1 field - raw data'!C6</f>
+        <v>95.162962508470898</v>
+      </c>
+      <c r="C7" s="13">
+        <f>'Table 1 field - raw data'!C13</f>
+        <v>69.488025912483195</v>
+      </c>
+      <c r="D7" s="14">
+        <f>'Table 1 field - raw data'!B6</f>
+        <v>-11.9</v>
+      </c>
+      <c r="E7" s="15">
+        <f>'Table 1 field - raw data'!B13</f>
+        <v>-13.3</v>
+      </c>
+      <c r="F7" s="16">
+        <f>'Table 1 field - raw data'!E6</f>
+        <v>0.956205473395907</v>
+      </c>
+      <c r="G7" s="17">
+        <f>'Table 1 field - raw data'!E13</f>
+        <v>1.3824169820843699</v>
+      </c>
+      <c r="H7" s="16">
+        <f>'Table 1 field - raw data'!D6</f>
+        <v>0.41071267036243903</v>
+      </c>
+      <c r="I7" s="17">
+        <f>'Table 1 field - raw data'!D13</f>
+        <v>0.59867515216147105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="19">
+        <f>'Table 1 field - raw data'!C7</f>
+        <v>182.213076546927</v>
+      </c>
+      <c r="C8" s="20">
+        <f>'Table 1 field - raw data'!C14</f>
+        <v>158.13699958153001</v>
+      </c>
+      <c r="D8" s="21">
+        <f>'Table 1 field - raw data'!B7</f>
+        <v>47.5</v>
+      </c>
+      <c r="E8" s="22">
+        <f>'Table 1 field - raw data'!B14</f>
+        <v>41.8</v>
+      </c>
+      <c r="F8" s="23">
+        <f>'Table 1 field - raw data'!E7</f>
+        <v>0.81353933321874194</v>
+      </c>
+      <c r="G8" s="24">
+        <f>'Table 1 field - raw data'!E14</f>
+        <v>0.98572691346165997</v>
+      </c>
+      <c r="H8" s="23">
+        <f>'Table 1 field - raw data'!D7</f>
+        <v>0.37127104234382302</v>
+      </c>
+      <c r="I8" s="24">
+        <f>'Table 1 field - raw data'!D14</f>
+        <v>0.46760521039555097</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="33">
+        <f>'Table 1 field - raw data'!C8</f>
+        <v>96.040602314077503</v>
+      </c>
+      <c r="C9" s="34">
+        <f>'Table 1 field - raw data'!C15</f>
+        <v>51.885675813081001</v>
+      </c>
+      <c r="D9" s="35">
+        <f>'Table 1 field - raw data'!B8</f>
+        <v>10.8</v>
+      </c>
+      <c r="E9" s="36">
+        <f>'Table 1 field - raw data'!B15</f>
+        <v>6.5</v>
+      </c>
+      <c r="F9" s="37">
+        <f>'Table 1 field - raw data'!E8</f>
+        <v>0.65032885421767295</v>
+      </c>
+      <c r="G9" s="38">
+        <f>'Table 1 field - raw data'!E15</f>
+        <v>1.03324963192462</v>
+      </c>
+      <c r="H9" s="37">
+        <f>'Table 1 field - raw data'!D8</f>
+        <v>0.47145600078347299</v>
+      </c>
+      <c r="I9" s="38">
+        <f>'Table 1 field - raw data'!D15</f>
+        <v>0.75673728770078996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="39">
+        <f>AVERAGE(B3:B9)</f>
+        <v>114.52131559438008</v>
+      </c>
+      <c r="C10" s="40">
+        <f t="shared" ref="C10:I10" si="0">AVERAGE(C3:C9)</f>
+        <v>85.519113006184099</v>
+      </c>
+      <c r="D10" s="41">
+        <f t="shared" si="0"/>
+        <v>6.7000000000000011</v>
+      </c>
+      <c r="E10" s="42">
+        <f t="shared" si="0"/>
+        <v>3.2285714285714278</v>
+      </c>
+      <c r="F10" s="43">
+        <f t="shared" si="0"/>
+        <v>0.78812026805630586</v>
+      </c>
+      <c r="G10" s="44">
+        <f t="shared" si="0"/>
+        <v>1.1412182961869524</v>
+      </c>
+      <c r="H10" s="43">
+        <f t="shared" si="0"/>
+        <v>0.45457279753251312</v>
+      </c>
+      <c r="I10" s="44">
+        <f t="shared" si="0"/>
+        <v>0.66549232436458383</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="C2">
+        <v>46.8</v>
+      </c>
+      <c r="D2">
+        <v>50.6</v>
+      </c>
+      <c r="E2">
+        <v>1.3264925760619399</v>
+      </c>
+      <c r="F2">
+        <v>0.94977537606193996</v>
+      </c>
+      <c r="G2">
+        <v>1.1936025751473101</v>
+      </c>
+      <c r="H2">
+        <v>0.70722325678104503</v>
+      </c>
+      <c r="I2">
+        <v>0.69082503808143803</v>
+      </c>
+      <c r="J2">
+        <v>0.31761842437134202</v>
+      </c>
+      <c r="K2">
+        <v>0.40690748489495798</v>
+      </c>
+      <c r="L2">
+        <v>0.43274806461895099</v>
+      </c>
+      <c r="M2">
+        <v>0.22662206988995201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>108.6</v>
+      </c>
+      <c r="C3">
+        <v>98.5</v>
+      </c>
+      <c r="D3">
+        <v>91.5</v>
+      </c>
+      <c r="E3">
+        <v>2.2049506480619399</v>
+      </c>
+      <c r="F3">
+        <v>2.00024414806194</v>
+      </c>
+      <c r="G3">
+        <v>1.85773088406194</v>
+      </c>
+      <c r="H3">
+        <v>0.96546512071329205</v>
+      </c>
+      <c r="I3">
+        <v>0.87769876929967305</v>
+      </c>
+      <c r="J3">
+        <v>0.63712450373597496</v>
+      </c>
+      <c r="K3">
+        <v>0.377574803193928</v>
+      </c>
+      <c r="L3">
+        <v>0.38775196783792598</v>
+      </c>
+      <c r="M3">
+        <v>0.28503364673370002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>75</v>
+      </c>
+      <c r="C4">
+        <v>67.5</v>
+      </c>
+      <c r="D4">
+        <v>60.2</v>
+      </c>
+      <c r="E4">
+        <v>1.5220841060619399</v>
+      </c>
+      <c r="F4">
+        <v>1.3702253440619401</v>
+      </c>
+      <c r="G4">
+        <v>1.2227832780619401</v>
+      </c>
+      <c r="H4">
+        <v>0.98047507399070599</v>
+      </c>
+      <c r="I4">
+        <v>0.93019406011203898</v>
+      </c>
+      <c r="J4">
+        <v>0.67053346789159896</v>
+      </c>
+      <c r="K4">
+        <v>0.41951285242667402</v>
+      </c>
+      <c r="L4">
+        <v>0.46811426299519598</v>
+      </c>
+      <c r="M4">
+        <v>0.33694581169332799</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>30.1</v>
+      </c>
+      <c r="C5">
+        <v>25.4</v>
+      </c>
+      <c r="D5">
+        <v>18.8</v>
+      </c>
+      <c r="E5">
+        <v>0.83586382093317102</v>
+      </c>
+      <c r="F5">
+        <v>0.60332796572881597</v>
+      </c>
+      <c r="G5">
+        <v>0.88872024081419099</v>
+      </c>
+      <c r="H5">
+        <v>0.95987013370315999</v>
+      </c>
+      <c r="I5">
+        <v>0.88673729685160996</v>
+      </c>
+      <c r="J5">
+        <v>0.71027998243946699</v>
+      </c>
+      <c r="K5">
+        <v>0.35680908719869198</v>
+      </c>
+      <c r="L5">
+        <v>0.39691877484075699</v>
+      </c>
+      <c r="M5">
+        <v>0.30625140776853899</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>63</v>
+      </c>
+      <c r="C6">
+        <v>54.8</v>
+      </c>
+      <c r="D6">
+        <v>49.4</v>
+      </c>
+      <c r="E6">
+        <v>1.2791523360619399</v>
+      </c>
+      <c r="F6">
+        <v>1.11282718006194</v>
+      </c>
+      <c r="G6">
+        <v>1.0036873200619401</v>
+      </c>
+      <c r="H6">
+        <v>0.97827409490972295</v>
+      </c>
+      <c r="I6">
+        <v>0.91565097784484495</v>
+      </c>
+      <c r="J6">
+        <v>0.64345323564458301</v>
+      </c>
+      <c r="K6">
+        <v>0.417700106510139</v>
+      </c>
+      <c r="L6">
+        <v>0.46456133905040398</v>
+      </c>
+      <c r="M6">
+        <v>0.32831283047439103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>165.6</v>
+      </c>
+      <c r="C7">
+        <v>144.4</v>
+      </c>
+      <c r="D7">
+        <v>149.9</v>
+      </c>
+      <c r="E7">
+        <v>3.3609131600619402</v>
+      </c>
+      <c r="F7">
+        <v>2.9305214960619401</v>
+      </c>
+      <c r="G7">
+        <v>3.0432672320619401</v>
+      </c>
+      <c r="H7">
+        <v>0.98400599280103296</v>
+      </c>
+      <c r="I7">
+        <v>0.93078577029168597</v>
+      </c>
+      <c r="J7">
+        <v>0.568102088811406</v>
+      </c>
+      <c r="K7">
+        <v>0.54931383902197095</v>
+      </c>
+      <c r="L7">
+        <v>0.60926055216130204</v>
+      </c>
+      <c r="M7">
+        <v>0.42013696880208601</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>48.7</v>
+      </c>
+      <c r="C8">
+        <v>60.5</v>
+      </c>
+      <c r="D8">
+        <v>33.9</v>
+      </c>
+      <c r="E8">
+        <v>0.98815472206193999</v>
+      </c>
+      <c r="F8">
+        <v>1.2283358760619401</v>
+      </c>
+      <c r="G8">
+        <v>0.86337590372881601</v>
+      </c>
+      <c r="H8">
+        <v>0.96972039389537301</v>
+      </c>
+      <c r="I8">
+        <v>0.90988591409012798</v>
+      </c>
+      <c r="J8">
+        <v>0.69401816999657095</v>
+      </c>
+      <c r="K8">
+        <v>0.441917209407449</v>
+      </c>
+      <c r="L8">
+        <v>0.48907248286788402</v>
+      </c>
+      <c r="M8">
+        <v>0.37111742539425402</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174954FC-3560-46B8-875C-4291803A546D}">
   <dimension ref="A1:N10"/>
   <sheetViews>
@@ -1913,26 +2591,26 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91" t="s">
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91" t="s">
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91" t="s">
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -2423,7 +3101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C7C311-7D6D-4A32-8A9D-56902DB428D3}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -2574,7 +3252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926FA25B-0675-4415-9EAE-A1DBC10ABC93}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -2759,7 +3437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BDAD93-B6AB-4202-9CA1-EDDEC2C0863F}">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -2937,11 +3615,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277FF2F4-7C15-432E-B910-25206B0CD439}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2954,22 +3632,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91" t="s">
+      <c r="C1" s="93"/>
+      <c r="D1" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91" t="s">
+      <c r="E1" s="93"/>
+      <c r="F1" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91" t="s">
+      <c r="G1" s="93"/>
+      <c r="H1" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="91"/>
+      <c r="I1" s="93"/>
     </row>
     <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -2999,7 +3677,6 @@
       <c r="I2" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="94"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -3037,45 +3714,44 @@
         <f>'Table 2 - copy raw data here'!C4</f>
         <v>0.70779926969762696</v>
       </c>
-      <c r="J3" s="95"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="97">
+      <c r="B4" s="61">
         <f>'Table 2 - copy raw data here'!F2</f>
         <v>76.751509380900899</v>
       </c>
-      <c r="C4" s="98">
+      <c r="C4" s="23">
         <f>'Table 2 - copy raw data here'!F4</f>
         <v>94.369071496377998</v>
       </c>
-      <c r="D4" s="99">
+      <c r="D4" s="91">
         <f>'Table 2 - copy raw data here'!E2/100</f>
         <v>0.22600000000000001</v>
       </c>
-      <c r="E4" s="100">
+      <c r="E4" s="92">
         <f>'Table 2 - copy raw data here'!E4/100</f>
         <v>0.18600000000000003</v>
       </c>
-      <c r="F4" s="97">
+      <c r="F4" s="61">
         <f>'Table 2 - copy raw data here'!H2</f>
         <v>0.47054979580306799</v>
       </c>
-      <c r="G4" s="98">
+      <c r="G4" s="23">
         <f>'Table 2 - copy raw data here'!H4</f>
         <v>0.43336244477795999</v>
       </c>
-      <c r="H4" s="97">
+      <c r="H4" s="61">
         <f>'Table 2 - copy raw data here'!G2</f>
         <v>0.28668293777689102</v>
       </c>
-      <c r="I4" s="98">
+      <c r="I4" s="23">
         <f>'Table 2 - copy raw data here'!G4</f>
         <v>0.22820097195871999</v>
       </c>
-      <c r="J4" s="94"/>
     </row>
     <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -3113,45 +3789,43 @@
         <f>'Table 2 - copy raw data here'!C5</f>
         <v>0.81001165098677397</v>
       </c>
-      <c r="J5" s="94"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="97">
+      <c r="B6" s="61">
         <f>'Table 2 - copy raw data here'!F3</f>
         <v>59.939262070064899</v>
       </c>
-      <c r="C6" s="98">
+      <c r="C6" s="23">
         <f>'Table 2 - copy raw data here'!F5</f>
         <v>73.845129344872603</v>
       </c>
-      <c r="D6" s="99">
+      <c r="D6" s="91">
         <f>'Table 2 - copy raw data here'!E3/100</f>
         <v>0.22699999999999998</v>
       </c>
-      <c r="E6" s="100">
+      <c r="E6" s="92">
         <f>'Table 2 - copy raw data here'!E5/100</f>
         <v>0.20600000000000002</v>
       </c>
-      <c r="F6" s="97">
+      <c r="F6" s="61">
         <f>'Table 2 - copy raw data here'!H3</f>
         <v>0.14339776384528699</v>
       </c>
-      <c r="G6" s="98">
+      <c r="G6" s="23">
         <f>'Table 2 - copy raw data here'!H5</f>
         <v>0.57062687867151096</v>
       </c>
-      <c r="H6" s="97">
+      <c r="H6" s="61">
         <f>'Table 2 - copy raw data here'!G3</f>
         <v>1.08667372563574E-2</v>
       </c>
-      <c r="I6" s="98">
+      <c r="I6" s="23">
         <f>'Table 2 - copy raw data here'!G5</f>
         <v>0.24506990273941801</v>
       </c>
-      <c r="J6" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3162,690 +3836,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08A1325-ED28-4898-AD5B-BD59E01EE5C5}">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>14.7</v>
-      </c>
-      <c r="C2">
-        <v>145.63510790120901</v>
-      </c>
-      <c r="D2">
-        <v>0.16558424807591199</v>
-      </c>
-      <c r="E2">
-        <v>0.47014517086380903</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>53</v>
-      </c>
-      <c r="C3">
-        <v>222.54464309897301</v>
-      </c>
-      <c r="D3">
-        <v>0.159415768085021</v>
-      </c>
-      <c r="E3">
-        <v>0.32618257824870001</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="C4">
-        <v>142.75054632827599</v>
-      </c>
-      <c r="D4">
-        <v>0.199570171231125</v>
-      </c>
-      <c r="E4">
-        <v>0.52362784643197202</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>-29.5</v>
-      </c>
-      <c r="C5">
-        <v>157.47284111953701</v>
-      </c>
-      <c r="D5">
-        <v>0.21098245367756199</v>
-      </c>
-      <c r="E5">
-        <v>0.54043995425047398</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>-0.9</v>
-      </c>
-      <c r="C6">
-        <v>139.66097462927701</v>
-      </c>
-      <c r="D6">
-        <v>0.113886370151475</v>
-      </c>
-      <c r="E6">
-        <v>0.46981089329105102</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>72.400000000000006</v>
-      </c>
-      <c r="C7">
-        <v>279.56460329244601</v>
-      </c>
-      <c r="D7">
-        <v>6.15220402826121E-2</v>
-      </c>
-      <c r="E7">
-        <v>0.27856920003521501</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>16.7</v>
-      </c>
-      <c r="C8">
-        <v>144.341525553043</v>
-      </c>
-      <c r="D8">
-        <v>0.24086493137075801</v>
-      </c>
-      <c r="E8">
-        <v>0.48963860411815502</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>12.2</v>
-      </c>
-      <c r="C9">
-        <v>98.874492262887699</v>
-      </c>
-      <c r="D9">
-        <v>0.35674008376359601</v>
-      </c>
-      <c r="E9">
-        <v>0.87094991566539404</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>49.6</v>
-      </c>
-      <c r="C10">
-        <v>190.131853581462</v>
-      </c>
-      <c r="D10">
-        <v>0.424228374684327</v>
-      </c>
-      <c r="E10">
-        <v>0.72327523984244202</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>14.4</v>
-      </c>
-      <c r="C11">
-        <v>99.603747299688393</v>
-      </c>
-      <c r="D11">
-        <v>0.39908717943623601</v>
-      </c>
-      <c r="E11">
-        <v>0.94534026810471095</v>
-      </c>
-      <c r="F11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>-31.3</v>
-      </c>
-      <c r="C12">
-        <v>123.92817748618199</v>
-      </c>
-      <c r="D12">
-        <v>0.373040091440559</v>
-      </c>
-      <c r="E12">
-        <v>0.89084759779255096</v>
-      </c>
-      <c r="F12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>-3.3</v>
-      </c>
-      <c r="C13">
-        <v>101.649558801711</v>
-      </c>
-      <c r="D13">
-        <v>0.169274581569167</v>
-      </c>
-      <c r="E13">
-        <v>0.649411350496922</v>
-      </c>
-      <c r="F13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>68.2</v>
-      </c>
-      <c r="C14">
-        <v>258.99252047032201</v>
-      </c>
-      <c r="D14">
-        <v>0.12538173855728399</v>
-      </c>
-      <c r="E14">
-        <v>0.51385254197861896</v>
-      </c>
-      <c r="F14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>14.4</v>
-      </c>
-      <c r="C15">
-        <v>89.848002117268393</v>
-      </c>
-      <c r="D15">
-        <v>0.56024285483421699</v>
-      </c>
-      <c r="E15">
-        <v>1.0560030090570101</v>
-      </c>
-      <c r="F15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC122BAA-6B80-44F9-A1DF-409EA6AE6532}">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="10" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="90"/>
-      <c r="B1" s="92" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="92" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="92" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="93"/>
-      <c r="H1" s="92" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="93"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="12">
-        <f>'Table 3 - copy raw data here'!C2</f>
-        <v>145.63510790120901</v>
-      </c>
-      <c r="C3" s="13">
-        <f>'Table 3 - copy raw data here'!C9</f>
-        <v>98.874492262887699</v>
-      </c>
-      <c r="D3" s="14">
-        <f>'Table 3 - copy raw data here'!B2</f>
-        <v>14.7</v>
-      </c>
-      <c r="E3" s="15">
-        <f>'Table 3 - copy raw data here'!B9</f>
-        <v>12.2</v>
-      </c>
-      <c r="F3" s="16">
-        <f>'Table 3 - copy raw data here'!E2</f>
-        <v>0.47014517086380903</v>
-      </c>
-      <c r="G3" s="17">
-        <f>'Table 3 - copy raw data here'!E9</f>
-        <v>0.87094991566539404</v>
-      </c>
-      <c r="H3" s="16">
-        <f>'Table 3 - copy raw data here'!D2</f>
-        <v>0.16558424807591199</v>
-      </c>
-      <c r="I3" s="17">
-        <f>'Table 3 - copy raw data here'!D9</f>
-        <v>0.35674008376359601</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="19">
-        <f>'Table 3 - copy raw data here'!C3</f>
-        <v>222.54464309897301</v>
-      </c>
-      <c r="C4" s="20">
-        <f>'Table 3 - copy raw data here'!C10</f>
-        <v>190.131853581462</v>
-      </c>
-      <c r="D4" s="21">
-        <f>'Table 3 - copy raw data here'!B3</f>
-        <v>53</v>
-      </c>
-      <c r="E4" s="22">
-        <f>'Table 3 - copy raw data here'!B10</f>
-        <v>49.6</v>
-      </c>
-      <c r="F4" s="23">
-        <f>'Table 3 - copy raw data here'!E3</f>
-        <v>0.32618257824870001</v>
-      </c>
-      <c r="G4" s="24">
-        <f>'Table 3 - copy raw data here'!E10</f>
-        <v>0.72327523984244202</v>
-      </c>
-      <c r="H4" s="23">
-        <f>'Table 3 - copy raw data here'!D3</f>
-        <v>0.159415768085021</v>
-      </c>
-      <c r="I4" s="24">
-        <f>'Table 3 - copy raw data here'!D10</f>
-        <v>0.424228374684327</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="12">
-        <f>'Table 3 - copy raw data here'!C4</f>
-        <v>142.75054632827599</v>
-      </c>
-      <c r="C5" s="13">
-        <f>'Table 3 - copy raw data here'!C11</f>
-        <v>99.603747299688393</v>
-      </c>
-      <c r="D5" s="14">
-        <f>'Table 3 - copy raw data here'!B4</f>
-        <v>16.899999999999999</v>
-      </c>
-      <c r="E5" s="15">
-        <f>'Table 3 - copy raw data here'!B11</f>
-        <v>14.4</v>
-      </c>
-      <c r="F5" s="16">
-        <f>'Table 3 - copy raw data here'!E4</f>
-        <v>0.52362784643197202</v>
-      </c>
-      <c r="G5" s="17">
-        <f>'Table 3 - copy raw data here'!E11</f>
-        <v>0.94534026810471095</v>
-      </c>
-      <c r="H5" s="16">
-        <f>'Table 3 - copy raw data here'!D4</f>
-        <v>0.199570171231125</v>
-      </c>
-      <c r="I5" s="17">
-        <f>'Table 3 - copy raw data here'!D11</f>
-        <v>0.39908717943623601</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="19">
-        <f>'Table 3 - copy raw data here'!C5</f>
-        <v>157.47284111953701</v>
-      </c>
-      <c r="C6" s="20">
-        <f>'Table 3 - copy raw data here'!C12</f>
-        <v>123.92817748618199</v>
-      </c>
-      <c r="D6" s="21">
-        <f>'Table 3 - copy raw data here'!B5</f>
-        <v>-29.5</v>
-      </c>
-      <c r="E6" s="22">
-        <f>'Table 3 - copy raw data here'!B12</f>
-        <v>-31.3</v>
-      </c>
-      <c r="F6" s="23">
-        <f>'Table 3 - copy raw data here'!E5</f>
-        <v>0.54043995425047398</v>
-      </c>
-      <c r="G6" s="24">
-        <f>'Table 3 - copy raw data here'!E12</f>
-        <v>0.89084759779255096</v>
-      </c>
-      <c r="H6" s="23">
-        <f>'Table 3 - copy raw data here'!D5</f>
-        <v>0.21098245367756199</v>
-      </c>
-      <c r="I6" s="24">
-        <f>'Table 3 - copy raw data here'!D12</f>
-        <v>0.373040091440559</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="12">
-        <f>'Table 3 - copy raw data here'!C6</f>
-        <v>139.66097462927701</v>
-      </c>
-      <c r="C7" s="13">
-        <f>'Table 3 - copy raw data here'!C13</f>
-        <v>101.649558801711</v>
-      </c>
-      <c r="D7" s="14">
-        <f>'Table 3 - copy raw data here'!B6</f>
-        <v>-0.9</v>
-      </c>
-      <c r="E7" s="15">
-        <f>'Table 3 - copy raw data here'!B13</f>
-        <v>-3.3</v>
-      </c>
-      <c r="F7" s="16">
-        <f>'Table 3 - copy raw data here'!E6</f>
-        <v>0.46981089329105102</v>
-      </c>
-      <c r="G7" s="17">
-        <f>'Table 3 - copy raw data here'!E13</f>
-        <v>0.649411350496922</v>
-      </c>
-      <c r="H7" s="16">
-        <f>'Table 3 - copy raw data here'!D6</f>
-        <v>0.113886370151475</v>
-      </c>
-      <c r="I7" s="17">
-        <f>'Table 3 - copy raw data here'!D13</f>
-        <v>0.169274581569167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="19">
-        <f>'Table 3 - copy raw data here'!C7</f>
-        <v>279.56460329244601</v>
-      </c>
-      <c r="C8" s="20">
-        <f>'Table 3 - copy raw data here'!C14</f>
-        <v>258.99252047032201</v>
-      </c>
-      <c r="D8" s="21">
-        <f>'Table 3 - copy raw data here'!B7</f>
-        <v>72.400000000000006</v>
-      </c>
-      <c r="E8" s="22">
-        <f>'Table 3 - copy raw data here'!B14</f>
-        <v>68.2</v>
-      </c>
-      <c r="F8" s="23">
-        <f>'Table 3 - copy raw data here'!E7</f>
-        <v>0.27856920003521501</v>
-      </c>
-      <c r="G8" s="24">
-        <f>'Table 3 - copy raw data here'!E14</f>
-        <v>0.51385254197861896</v>
-      </c>
-      <c r="H8" s="23">
-        <f>'Table 3 - copy raw data here'!D7</f>
-        <v>6.15220402826121E-2</v>
-      </c>
-      <c r="I8" s="24">
-        <f>'Table 3 - copy raw data here'!D14</f>
-        <v>0.12538173855728399</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="33">
-        <f>'Table 3 - copy raw data here'!C8</f>
-        <v>144.341525553043</v>
-      </c>
-      <c r="C9" s="34">
-        <f>'Table 3 - copy raw data here'!C15</f>
-        <v>89.848002117268393</v>
-      </c>
-      <c r="D9" s="35">
-        <f>'Table 3 - copy raw data here'!B8</f>
-        <v>16.7</v>
-      </c>
-      <c r="E9" s="36">
-        <f>'Table 3 - copy raw data here'!B15</f>
-        <v>14.4</v>
-      </c>
-      <c r="F9" s="37">
-        <f>'Table 3 - copy raw data here'!E8</f>
-        <v>0.48963860411815502</v>
-      </c>
-      <c r="G9" s="38">
-        <f>'Table 3 - copy raw data here'!E15</f>
-        <v>1.0560030090570101</v>
-      </c>
-      <c r="H9" s="37">
-        <f>'Table 3 - copy raw data here'!D8</f>
-        <v>0.24086493137075801</v>
-      </c>
-      <c r="I9" s="38">
-        <f>'Table 3 - copy raw data here'!D15</f>
-        <v>0.56024285483421699</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="39">
-        <f>AVERAGE(B3:B9)</f>
-        <v>175.99574884610871</v>
-      </c>
-      <c r="C10" s="40">
-        <f t="shared" ref="C10:I10" si="0">AVERAGE(C3:C9)</f>
-        <v>137.57547885993162</v>
-      </c>
-      <c r="D10" s="41">
-        <f t="shared" si="0"/>
-        <v>20.471428571428568</v>
-      </c>
-      <c r="E10" s="42">
-        <f t="shared" si="0"/>
-        <v>17.742857142857144</v>
-      </c>
-      <c r="F10" s="43">
-        <f t="shared" si="0"/>
-        <v>0.44263060674848231</v>
-      </c>
-      <c r="G10" s="44">
-        <f t="shared" si="0"/>
-        <v>0.80709713184823573</v>
-      </c>
-      <c r="H10" s="43">
-        <f t="shared" si="0"/>
-        <v>0.16454656898206643</v>
-      </c>
-      <c r="I10" s="44">
-        <f t="shared" si="0"/>
-        <v>0.34399927204076947</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update WRG figures and tables
</commit_message>
<xml_diff>
--- a/figures+tables/Tables_FitStats_Formatted.xlsx
+++ b/figures+tables/Tables_FitStats_Formatted.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s947z036\WorkGits\SD-6_MapWaterConservation\figures+tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C965C74-7257-4432-AAA4-949D1755E81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28114DB8-175E-4E8D-A7C9-30A3079D128E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 field - raw data" sheetId="5" r:id="rId1"/>
     <sheet name="Table 1 field - formatted" sheetId="6" r:id="rId2"/>
-    <sheet name="Table 1 - copy raw data here" sheetId="1" r:id="rId3"/>
-    <sheet name="Table 1 formatted" sheetId="3" r:id="rId4"/>
-    <sheet name="Table S1 copy raw data" sheetId="7" r:id="rId5"/>
-    <sheet name="Table S1 Precip corrected table" sheetId="4" r:id="rId6"/>
-    <sheet name="Table 2 - copy raw data here" sheetId="10" r:id="rId7"/>
-    <sheet name="Table 2 formatted" sheetId="11" r:id="rId8"/>
+    <sheet name="Table 2 WRG - raw data" sheetId="10" r:id="rId3"/>
+    <sheet name="Table 2 WRG - formatted" sheetId="11" r:id="rId4"/>
+    <sheet name="Table 1 - copy raw data here" sheetId="1" r:id="rId5"/>
+    <sheet name="Table 1 formatted" sheetId="3" r:id="rId6"/>
+    <sheet name="Table S1 copy raw data" sheetId="7" r:id="rId7"/>
+    <sheet name="Table S1 Precip corrected table" sheetId="4" r:id="rId8"/>
     <sheet name="Table S2 - copy raw data here" sheetId="8" r:id="rId9"/>
     <sheet name="Table S2 formatted" sheetId="9" r:id="rId10"/>
   </sheets>
@@ -886,13 +886,13 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1178,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08A1325-ED28-4898-AD5B-BD59E01EE5C5}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -1505,22 +1505,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="95"/>
-      <c r="D1" s="94" t="s">
+      <c r="C1" s="94"/>
+      <c r="D1" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="95"/>
-      <c r="F1" s="94" t="s">
+      <c r="E1" s="94"/>
+      <c r="F1" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="95"/>
-      <c r="H1" s="94" t="s">
+      <c r="G1" s="94"/>
+      <c r="H1" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="95"/>
+      <c r="I1" s="94"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -1874,22 +1874,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="90"/>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="95"/>
-      <c r="D1" s="94" t="s">
+      <c r="C1" s="94"/>
+      <c r="D1" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="95"/>
-      <c r="F1" s="94" t="s">
+      <c r="E1" s="94"/>
+      <c r="F1" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="95"/>
-      <c r="H1" s="94" t="s">
+      <c r="G1" s="94"/>
+      <c r="H1" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="95"/>
+      <c r="I1" s="94"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -2228,6 +2228,408 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BDAD93-B6AB-4202-9CA1-EDDEC2C0863F}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>69.3</v>
+      </c>
+      <c r="B2">
+        <v>1.0669017868541999</v>
+      </c>
+      <c r="C2">
+        <v>0.72116030657730201</v>
+      </c>
+      <c r="D2">
+        <v>0.498102024152836</v>
+      </c>
+      <c r="E2">
+        <v>22.6</v>
+      </c>
+      <c r="F2">
+        <v>76.751509380900899</v>
+      </c>
+      <c r="G2">
+        <v>0.28668293777689102</v>
+      </c>
+      <c r="H2">
+        <v>0.47054979580306799</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>69.3</v>
+      </c>
+      <c r="B3">
+        <v>1.03156852648598</v>
+      </c>
+      <c r="C3">
+        <v>0.79830091181460205</v>
+      </c>
+      <c r="D3">
+        <v>0.53288739442773103</v>
+      </c>
+      <c r="E3">
+        <v>22.7</v>
+      </c>
+      <c r="F3">
+        <v>59.939262070064899</v>
+      </c>
+      <c r="G3">
+        <v>1.08667372563574E-2</v>
+      </c>
+      <c r="H3">
+        <v>0.14339776384528699</v>
+      </c>
+      <c r="I3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>0.66340200734979504</v>
+      </c>
+      <c r="C4">
+        <v>0.70779926969762696</v>
+      </c>
+      <c r="D4">
+        <v>0.60573248792935397</v>
+      </c>
+      <c r="E4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="F4">
+        <v>94.369071496377998</v>
+      </c>
+      <c r="G4">
+        <v>0.22820097195871999</v>
+      </c>
+      <c r="H4">
+        <v>0.43336244477795999</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>31.4</v>
+      </c>
+      <c r="B5">
+        <v>0.61310432417045002</v>
+      </c>
+      <c r="C5">
+        <v>0.81001165098677397</v>
+      </c>
+      <c r="D5">
+        <v>0.64269987881578905</v>
+      </c>
+      <c r="E5">
+        <v>20.6</v>
+      </c>
+      <c r="F5">
+        <v>73.845129344872603</v>
+      </c>
+      <c r="G5">
+        <v>0.24506990273941801</v>
+      </c>
+      <c r="H5">
+        <v>0.57062687867151096</v>
+      </c>
+      <c r="I5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277FF2F4-7C15-432E-B910-25206B0CD439}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="6.28515625" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="18"/>
+      <c r="B1" s="95" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="95"/>
+    </row>
+    <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="55">
+        <f>'Table 2 WRG - raw data'!B2</f>
+        <v>1.0669017868541999</v>
+      </c>
+      <c r="C3" s="56">
+        <f>'Table 2 WRG - raw data'!B4</f>
+        <v>0.66340200734979504</v>
+      </c>
+      <c r="D3" s="58">
+        <f>'Table 2 WRG - raw data'!A2/100</f>
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="E3" s="59">
+        <f>'Table 2 WRG - raw data'!A4/100</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F3" s="55">
+        <f>'Table 2 WRG - raw data'!D2</f>
+        <v>0.498102024152836</v>
+      </c>
+      <c r="G3" s="56">
+        <f>'Table 2 WRG - raw data'!D4</f>
+        <v>0.60573248792935397</v>
+      </c>
+      <c r="H3" s="55">
+        <f>'Table 2 WRG - raw data'!C2</f>
+        <v>0.72116030657730201</v>
+      </c>
+      <c r="I3" s="56">
+        <f>'Table 2 WRG - raw data'!C4</f>
+        <v>0.70779926969762696</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="61">
+        <f>'Table 2 WRG - raw data'!F2</f>
+        <v>76.751509380900899</v>
+      </c>
+      <c r="C4" s="23">
+        <f>'Table 2 WRG - raw data'!F4</f>
+        <v>94.369071496377998</v>
+      </c>
+      <c r="D4" s="91">
+        <f>'Table 2 WRG - raw data'!E2/100</f>
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="E4" s="92">
+        <f>'Table 2 WRG - raw data'!E4/100</f>
+        <v>0.18600000000000003</v>
+      </c>
+      <c r="F4" s="61">
+        <f>'Table 2 WRG - raw data'!H2</f>
+        <v>0.47054979580306799</v>
+      </c>
+      <c r="G4" s="23">
+        <f>'Table 2 WRG - raw data'!H4</f>
+        <v>0.43336244477795999</v>
+      </c>
+      <c r="H4" s="61">
+        <f>'Table 2 WRG - raw data'!G2</f>
+        <v>0.28668293777689102</v>
+      </c>
+      <c r="I4" s="23">
+        <f>'Table 2 WRG - raw data'!G4</f>
+        <v>0.22820097195871999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="65">
+        <f>'Table 2 WRG - raw data'!B3</f>
+        <v>1.03156852648598</v>
+      </c>
+      <c r="C5" s="16">
+        <f>'Table 2 WRG - raw data'!B5</f>
+        <v>0.61310432417045002</v>
+      </c>
+      <c r="D5" s="66">
+        <f>'Table 2 WRG - raw data'!A3/100</f>
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="E5" s="67">
+        <f>'Table 2 WRG - raw data'!A5/100</f>
+        <v>0.314</v>
+      </c>
+      <c r="F5" s="65">
+        <f>'Table 2 WRG - raw data'!D3</f>
+        <v>0.53288739442773103</v>
+      </c>
+      <c r="G5" s="16">
+        <f>'Table 2 WRG - raw data'!D5</f>
+        <v>0.64269987881578905</v>
+      </c>
+      <c r="H5" s="65">
+        <f>'Table 2 WRG - raw data'!C3</f>
+        <v>0.79830091181460205</v>
+      </c>
+      <c r="I5" s="16">
+        <f>'Table 2 WRG - raw data'!C5</f>
+        <v>0.81001165098677397</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="61">
+        <f>'Table 2 WRG - raw data'!F3</f>
+        <v>59.939262070064899</v>
+      </c>
+      <c r="C6" s="23">
+        <f>'Table 2 WRG - raw data'!F5</f>
+        <v>73.845129344872603</v>
+      </c>
+      <c r="D6" s="91">
+        <f>'Table 2 WRG - raw data'!E3/100</f>
+        <v>0.22699999999999998</v>
+      </c>
+      <c r="E6" s="92">
+        <f>'Table 2 WRG - raw data'!E5/100</f>
+        <v>0.20600000000000002</v>
+      </c>
+      <c r="F6" s="61">
+        <f>'Table 2 WRG - raw data'!H3</f>
+        <v>0.14339776384528699</v>
+      </c>
+      <c r="G6" s="23">
+        <f>'Table 2 WRG - raw data'!H5</f>
+        <v>0.57062687867151096</v>
+      </c>
+      <c r="H6" s="61">
+        <f>'Table 2 WRG - raw data'!G3</f>
+        <v>1.08667372563574E-2</v>
+      </c>
+      <c r="I6" s="23">
+        <f>'Table 2 WRG - raw data'!G5</f>
+        <v>0.24506990273941801</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
@@ -2574,7 +2976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174954FC-3560-46B8-875C-4291803A546D}">
   <dimension ref="A1:N10"/>
   <sheetViews>
@@ -2591,26 +2993,26 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93" t="s">
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93" t="s">
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93" t="s">
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -3101,7 +3503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C7C311-7D6D-4A32-8A9D-56902DB428D3}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -3252,7 +3654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926FA25B-0675-4415-9EAE-A1DBC10ABC93}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -3437,408 +3839,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BDAD93-B6AB-4202-9CA1-EDDEC2C0863F}">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>69.3</v>
-      </c>
-      <c r="B2">
-        <v>1.0669017868541999</v>
-      </c>
-      <c r="C2">
-        <v>0.72116030657730201</v>
-      </c>
-      <c r="D2">
-        <v>0.498102024152836</v>
-      </c>
-      <c r="E2">
-        <v>22.6</v>
-      </c>
-      <c r="F2">
-        <v>76.751509380900899</v>
-      </c>
-      <c r="G2">
-        <v>0.28668293777689102</v>
-      </c>
-      <c r="H2">
-        <v>0.47054979580306799</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>69.3</v>
-      </c>
-      <c r="B3">
-        <v>1.03156852648598</v>
-      </c>
-      <c r="C3">
-        <v>0.79830091181460205</v>
-      </c>
-      <c r="D3">
-        <v>0.53288739442773103</v>
-      </c>
-      <c r="E3">
-        <v>22.7</v>
-      </c>
-      <c r="F3">
-        <v>59.939262070064899</v>
-      </c>
-      <c r="G3">
-        <v>1.08667372563574E-2</v>
-      </c>
-      <c r="H3">
-        <v>0.14339776384528699</v>
-      </c>
-      <c r="I3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>28</v>
-      </c>
-      <c r="B4">
-        <v>0.66340200734979504</v>
-      </c>
-      <c r="C4">
-        <v>0.70779926969762696</v>
-      </c>
-      <c r="D4">
-        <v>0.60573248792935397</v>
-      </c>
-      <c r="E4">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="F4">
-        <v>94.369071496377998</v>
-      </c>
-      <c r="G4">
-        <v>0.22820097195871999</v>
-      </c>
-      <c r="H4">
-        <v>0.43336244477795999</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>31.4</v>
-      </c>
-      <c r="B5">
-        <v>0.61310432417045002</v>
-      </c>
-      <c r="C5">
-        <v>0.81001165098677397</v>
-      </c>
-      <c r="D5">
-        <v>0.64269987881578905</v>
-      </c>
-      <c r="E5">
-        <v>20.6</v>
-      </c>
-      <c r="F5">
-        <v>73.845129344872603</v>
-      </c>
-      <c r="G5">
-        <v>0.24506990273941801</v>
-      </c>
-      <c r="H5">
-        <v>0.57062687867151096</v>
-      </c>
-      <c r="I5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277FF2F4-7C15-432E-B910-25206B0CD439}">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="6.28515625" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="93" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="93"/>
-    </row>
-    <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="I2" s="53" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="55">
-        <f>'Table 2 - copy raw data here'!B2</f>
-        <v>1.0669017868541999</v>
-      </c>
-      <c r="C3" s="56">
-        <f>'Table 2 - copy raw data here'!B4</f>
-        <v>0.66340200734979504</v>
-      </c>
-      <c r="D3" s="58">
-        <f>'Table 2 - copy raw data here'!A2/100</f>
-        <v>0.69299999999999995</v>
-      </c>
-      <c r="E3" s="59">
-        <f>'Table 2 - copy raw data here'!A4/100</f>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F3" s="55">
-        <f>'Table 2 - copy raw data here'!D2</f>
-        <v>0.498102024152836</v>
-      </c>
-      <c r="G3" s="56">
-        <f>'Table 2 - copy raw data here'!D4</f>
-        <v>0.60573248792935397</v>
-      </c>
-      <c r="H3" s="55">
-        <f>'Table 2 - copy raw data here'!C2</f>
-        <v>0.72116030657730201</v>
-      </c>
-      <c r="I3" s="56">
-        <f>'Table 2 - copy raw data here'!C4</f>
-        <v>0.70779926969762696</v>
-      </c>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="61">
-        <f>'Table 2 - copy raw data here'!F2</f>
-        <v>76.751509380900899</v>
-      </c>
-      <c r="C4" s="23">
-        <f>'Table 2 - copy raw data here'!F4</f>
-        <v>94.369071496377998</v>
-      </c>
-      <c r="D4" s="91">
-        <f>'Table 2 - copy raw data here'!E2/100</f>
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="E4" s="92">
-        <f>'Table 2 - copy raw data here'!E4/100</f>
-        <v>0.18600000000000003</v>
-      </c>
-      <c r="F4" s="61">
-        <f>'Table 2 - copy raw data here'!H2</f>
-        <v>0.47054979580306799</v>
-      </c>
-      <c r="G4" s="23">
-        <f>'Table 2 - copy raw data here'!H4</f>
-        <v>0.43336244477795999</v>
-      </c>
-      <c r="H4" s="61">
-        <f>'Table 2 - copy raw data here'!G2</f>
-        <v>0.28668293777689102</v>
-      </c>
-      <c r="I4" s="23">
-        <f>'Table 2 - copy raw data here'!G4</f>
-        <v>0.22820097195871999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="65">
-        <f>'Table 2 - copy raw data here'!B3</f>
-        <v>1.03156852648598</v>
-      </c>
-      <c r="C5" s="16">
-        <f>'Table 2 - copy raw data here'!B5</f>
-        <v>0.61310432417045002</v>
-      </c>
-      <c r="D5" s="66">
-        <f>'Table 2 - copy raw data here'!A3/100</f>
-        <v>0.69299999999999995</v>
-      </c>
-      <c r="E5" s="67">
-        <f>'Table 2 - copy raw data here'!A5/100</f>
-        <v>0.314</v>
-      </c>
-      <c r="F5" s="65">
-        <f>'Table 2 - copy raw data here'!D3</f>
-        <v>0.53288739442773103</v>
-      </c>
-      <c r="G5" s="16">
-        <f>'Table 2 - copy raw data here'!D5</f>
-        <v>0.64269987881578905</v>
-      </c>
-      <c r="H5" s="65">
-        <f>'Table 2 - copy raw data here'!C3</f>
-        <v>0.79830091181460205</v>
-      </c>
-      <c r="I5" s="16">
-        <f>'Table 2 - copy raw data here'!C5</f>
-        <v>0.81001165098677397</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="61">
-        <f>'Table 2 - copy raw data here'!F3</f>
-        <v>59.939262070064899</v>
-      </c>
-      <c r="C6" s="23">
-        <f>'Table 2 - copy raw data here'!F5</f>
-        <v>73.845129344872603</v>
-      </c>
-      <c r="D6" s="91">
-        <f>'Table 2 - copy raw data here'!E3/100</f>
-        <v>0.22699999999999998</v>
-      </c>
-      <c r="E6" s="92">
-        <f>'Table 2 - copy raw data here'!E5/100</f>
-        <v>0.20600000000000002</v>
-      </c>
-      <c r="F6" s="61">
-        <f>'Table 2 - copy raw data here'!H3</f>
-        <v>0.14339776384528699</v>
-      </c>
-      <c r="G6" s="23">
-        <f>'Table 2 - copy raw data here'!H5</f>
-        <v>0.57062687867151096</v>
-      </c>
-      <c r="H6" s="61">
-        <f>'Table 2 - copy raw data here'!G3</f>
-        <v>1.08667372563574E-2</v>
-      </c>
-      <c r="I6" s="23">
-        <f>'Table 2 - copy raw data here'!G5</f>
-        <v>0.24506990273941801</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3187032F-1B6C-4E62-935E-29A85F8C99C3}">
   <dimension ref="A1:F15"/>

</xml_diff>

<commit_message>
Update all calculations based on IrrigatedPrc field
</commit_message>
<xml_diff>
--- a/figures+tables/Tables_FitStats_Formatted.xlsx
+++ b/figures+tables/Tables_FitStats_Formatted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s947z036\WorkGits\SD-6_MapWaterConservation\figures+tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2942C6FE-5EAC-43FD-A2DD-FC4A7658F0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133BE435-C7CF-40C8-A461-FB7F30FE0D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 field - raw data" sheetId="5" r:id="rId1"/>
@@ -826,15 +826,6 @@
     <xf numFmtId="2" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -843,6 +834,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1454,22 +1454,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="79" t="s">
+      <c r="C1" s="83"/>
+      <c r="D1" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="80"/>
-      <c r="F1" s="79" t="s">
+      <c r="E1" s="83"/>
+      <c r="F1" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="80"/>
-      <c r="H1" s="79" t="s">
+      <c r="G1" s="83"/>
+      <c r="H1" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="80"/>
+      <c r="I1" s="83"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1823,22 +1823,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="68"/>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="79" t="s">
+      <c r="C1" s="83"/>
+      <c r="D1" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="80"/>
-      <c r="F1" s="79" t="s">
+      <c r="E1" s="83"/>
+      <c r="F1" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="80"/>
-      <c r="H1" s="79" t="s">
+      <c r="G1" s="83"/>
+      <c r="H1" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="80"/>
+      <c r="I1" s="83"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2223,28 +2223,28 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>69.3</v>
+        <v>57</v>
       </c>
       <c r="B2">
-        <v>1.0669017868541999</v>
+        <v>0.91518275790176495</v>
       </c>
       <c r="C2">
-        <v>0.72116030657730201</v>
+        <v>0.71888166334803105</v>
       </c>
       <c r="D2">
-        <v>0.498102024152836</v>
+        <v>0.52909363703263701</v>
       </c>
       <c r="E2">
-        <v>22.6</v>
+        <v>41.9</v>
       </c>
       <c r="F2">
-        <v>76.751509380900899</v>
+        <v>98.759197343525599</v>
       </c>
       <c r="G2">
-        <v>0.28668293777689102</v>
+        <v>0.35484322928865197</v>
       </c>
       <c r="H2">
-        <v>0.47054979580306799</v>
+        <v>0.53539159921825896</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2255,28 +2255,28 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>69.3</v>
+        <v>57.1</v>
       </c>
       <c r="B3">
-        <v>1.03156852648598</v>
+        <v>0.86468561938909405</v>
       </c>
       <c r="C3">
-        <v>0.79830091181460205</v>
+        <v>0.79431290158147605</v>
       </c>
       <c r="D3">
-        <v>0.53288739442773103</v>
+        <v>0.56803530487022602</v>
       </c>
       <c r="E3">
-        <v>22.7</v>
+        <v>41.2</v>
       </c>
       <c r="F3">
-        <v>59.939262070064899</v>
+        <v>90.971653090639904</v>
       </c>
       <c r="G3">
-        <v>1.08667372563574E-2</v>
+        <v>5.2893106728812998E-2</v>
       </c>
       <c r="H3">
-        <v>0.14339776384528699</v>
+        <v>0.44300427827585298</v>
       </c>
       <c r="I3" t="s">
         <v>39</v>
@@ -2287,28 +2287,28 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>28</v>
+        <v>40.1</v>
       </c>
       <c r="B4">
-        <v>0.66340200734979504</v>
+        <v>0.66377243550112197</v>
       </c>
       <c r="C4">
-        <v>0.70779926969762696</v>
+        <v>0.82990617265505395</v>
       </c>
       <c r="D4">
-        <v>0.60573248792935397</v>
+        <v>0.64492231918432597</v>
       </c>
       <c r="E4">
-        <v>18.600000000000001</v>
+        <v>38.4</v>
       </c>
       <c r="F4">
-        <v>94.369071496377998</v>
+        <v>93.808825454358299</v>
       </c>
       <c r="G4">
-        <v>0.22820097195871999</v>
+        <v>0.40348024279047201</v>
       </c>
       <c r="H4">
-        <v>0.43336244477795999</v>
+        <v>0.55829468693486495</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
@@ -2319,28 +2319,28 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>31.4</v>
+        <v>41.3</v>
       </c>
       <c r="B5">
-        <v>0.61310432417045002</v>
+        <v>0.66948215809220002</v>
       </c>
       <c r="C5">
-        <v>0.81001165098677397</v>
+        <v>0.893584640723324</v>
       </c>
       <c r="D5">
-        <v>0.64269987881578905</v>
+        <v>0.68187133802716304</v>
       </c>
       <c r="E5">
-        <v>20.6</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="F5">
-        <v>73.845129344872603</v>
+        <v>89.8800460460008</v>
       </c>
       <c r="G5">
-        <v>0.24506990273941801</v>
+        <v>0.32447301864828998</v>
       </c>
       <c r="H5">
-        <v>0.57062687867151096</v>
+        <v>0.58431264657070303</v>
       </c>
       <c r="I5" t="s">
         <v>39</v>
@@ -2358,7 +2358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277FF2F4-7C15-432E-B910-25206B0CD439}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -2371,22 +2371,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81" t="s">
+      <c r="C1" s="84"/>
+      <c r="D1" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81" t="s">
+      <c r="E1" s="84"/>
+      <c r="F1" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81" t="s">
+      <c r="G1" s="84"/>
+      <c r="H1" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="81"/>
+      <c r="I1" s="84"/>
     </row>
     <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2423,35 +2423,35 @@
       </c>
       <c r="B3" s="51">
         <f>'Table 2 WRG - raw data'!B2</f>
-        <v>1.0669017868541999</v>
+        <v>0.91518275790176495</v>
       </c>
       <c r="C3" s="52">
         <f>'Table 2 WRG - raw data'!B4</f>
-        <v>0.66340200734979504</v>
+        <v>0.66377243550112197</v>
       </c>
       <c r="D3" s="54">
         <f>'Table 2 WRG - raw data'!A2/100</f>
-        <v>0.69299999999999995</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E3" s="55">
         <f>'Table 2 WRG - raw data'!A4/100</f>
-        <v>0.28000000000000003</v>
+        <v>0.40100000000000002</v>
       </c>
       <c r="F3" s="51">
         <f>'Table 2 WRG - raw data'!D2</f>
-        <v>0.498102024152836</v>
+        <v>0.52909363703263701</v>
       </c>
       <c r="G3" s="52">
         <f>'Table 2 WRG - raw data'!D4</f>
-        <v>0.60573248792935397</v>
+        <v>0.64492231918432597</v>
       </c>
       <c r="H3" s="51">
         <f>'Table 2 WRG - raw data'!C2</f>
-        <v>0.72116030657730201</v>
+        <v>0.71888166334803105</v>
       </c>
       <c r="I3" s="52">
         <f>'Table 2 WRG - raw data'!C4</f>
-        <v>0.70779926969762696</v>
+        <v>0.82990617265505395</v>
       </c>
       <c r="J3" s="2"/>
     </row>
@@ -2461,35 +2461,35 @@
       </c>
       <c r="B4" s="57">
         <f>'Table 2 WRG - raw data'!F2</f>
-        <v>76.751509380900899</v>
+        <v>98.759197343525599</v>
       </c>
       <c r="C4" s="20">
         <f>'Table 2 WRG - raw data'!F4</f>
-        <v>94.369071496377998</v>
+        <v>93.808825454358299</v>
       </c>
       <c r="D4" s="69">
         <f>'Table 2 WRG - raw data'!E2/100</f>
-        <v>0.22600000000000001</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="E4" s="70">
         <f>'Table 2 WRG - raw data'!E4/100</f>
-        <v>0.18600000000000003</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="F4" s="57">
         <f>'Table 2 WRG - raw data'!H2</f>
-        <v>0.47054979580306799</v>
+        <v>0.53539159921825896</v>
       </c>
       <c r="G4" s="20">
         <f>'Table 2 WRG - raw data'!H4</f>
-        <v>0.43336244477795999</v>
+        <v>0.55829468693486495</v>
       </c>
       <c r="H4" s="57">
         <f>'Table 2 WRG - raw data'!G2</f>
-        <v>0.28668293777689102</v>
+        <v>0.35484322928865197</v>
       </c>
       <c r="I4" s="20">
         <f>'Table 2 WRG - raw data'!G4</f>
-        <v>0.22820097195871999</v>
+        <v>0.40348024279047201</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -2498,35 +2498,35 @@
       </c>
       <c r="B5" s="61">
         <f>'Table 2 WRG - raw data'!B3</f>
-        <v>1.03156852648598</v>
+        <v>0.86468561938909405</v>
       </c>
       <c r="C5" s="13">
         <f>'Table 2 WRG - raw data'!B5</f>
-        <v>0.61310432417045002</v>
+        <v>0.66948215809220002</v>
       </c>
       <c r="D5" s="62">
         <f>'Table 2 WRG - raw data'!A3/100</f>
-        <v>0.69299999999999995</v>
+        <v>0.57100000000000006</v>
       </c>
       <c r="E5" s="63">
         <f>'Table 2 WRG - raw data'!A5/100</f>
-        <v>0.314</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="F5" s="61">
         <f>'Table 2 WRG - raw data'!D3</f>
-        <v>0.53288739442773103</v>
+        <v>0.56803530487022602</v>
       </c>
       <c r="G5" s="13">
         <f>'Table 2 WRG - raw data'!D5</f>
-        <v>0.64269987881578905</v>
+        <v>0.68187133802716304</v>
       </c>
       <c r="H5" s="61">
         <f>'Table 2 WRG - raw data'!C3</f>
-        <v>0.79830091181460205</v>
+        <v>0.79431290158147605</v>
       </c>
       <c r="I5" s="13">
         <f>'Table 2 WRG - raw data'!C5</f>
-        <v>0.81001165098677397</v>
+        <v>0.893584640723324</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2535,35 +2535,35 @@
       </c>
       <c r="B6" s="57">
         <f>'Table 2 WRG - raw data'!F3</f>
-        <v>59.939262070064899</v>
+        <v>90.971653090639904</v>
       </c>
       <c r="C6" s="20">
         <f>'Table 2 WRG - raw data'!F5</f>
-        <v>73.845129344872603</v>
+        <v>89.8800460460008</v>
       </c>
       <c r="D6" s="69">
         <f>'Table 2 WRG - raw data'!E3/100</f>
-        <v>0.22699999999999998</v>
+        <v>0.41200000000000003</v>
       </c>
       <c r="E6" s="70">
         <f>'Table 2 WRG - raw data'!E5/100</f>
-        <v>0.20600000000000002</v>
+        <v>0.39299999999999996</v>
       </c>
       <c r="F6" s="57">
         <f>'Table 2 WRG - raw data'!H3</f>
-        <v>0.14339776384528699</v>
+        <v>0.44300427827585298</v>
       </c>
       <c r="G6" s="20">
         <f>'Table 2 WRG - raw data'!H5</f>
-        <v>0.57062687867151096</v>
+        <v>0.58431264657070303</v>
       </c>
       <c r="H6" s="57">
         <f>'Table 2 WRG - raw data'!G3</f>
-        <v>1.08667372563574E-2</v>
+        <v>5.2893106728812998E-2</v>
       </c>
       <c r="I6" s="20">
         <f>'Table 2 WRG - raw data'!G5</f>
-        <v>0.24506990273941801</v>
+        <v>0.32447301864828998</v>
       </c>
     </row>
   </sheetData>
@@ -2583,7 +2583,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection sqref="A1:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2638,40 +2638,40 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>46.8</v>
+        <v>36</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>-6.9</v>
+        <v>26.6</v>
       </c>
       <c r="E2">
-        <v>0.94977537606193996</v>
+        <v>0.73191821373571997</v>
       </c>
       <c r="F2">
-        <v>0.340981905337637</v>
+        <v>0.346316575163579</v>
       </c>
       <c r="G2">
-        <v>0.29586560417854602</v>
+        <v>0.55283703019616603</v>
       </c>
       <c r="H2">
-        <v>0.69082503808143803</v>
+        <v>0.67812486552248197</v>
       </c>
       <c r="I2">
-        <v>0.46154690097069101</v>
+        <v>0.47227708829139098</v>
       </c>
       <c r="J2">
-        <v>0.69082503808143803</v>
+        <v>0.67812486552248197</v>
       </c>
       <c r="K2">
-        <v>0.43274806461895099</v>
+        <v>0.457202436971055</v>
       </c>
       <c r="L2">
-        <v>0.564953094661791</v>
+        <v>0.58091958959658196</v>
       </c>
       <c r="M2">
-        <v>0.68256792526648402</v>
+        <v>0.49108747257900598</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2679,40 +2679,40 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>98.5</v>
+        <v>83.9</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>25.9</v>
+        <v>71.2</v>
       </c>
       <c r="E3">
-        <v>2.00024414806194</v>
+        <v>1.7055407677357199</v>
       </c>
       <c r="F3">
-        <v>0.16927279982131699</v>
+        <v>0.182273254319129</v>
       </c>
       <c r="G3">
-        <v>0.52525984097393996</v>
+        <v>1.44758493082572</v>
       </c>
       <c r="H3">
-        <v>0.87769876929967305</v>
+        <v>0.86493595173328996</v>
       </c>
       <c r="I3">
-        <v>0.85119026125060704</v>
+        <v>0.82092275638951395</v>
       </c>
       <c r="J3">
-        <v>0.87769876929967305</v>
+        <v>0.86493595173328996</v>
       </c>
       <c r="K3">
-        <v>0.38775196783792598</v>
+        <v>0.41143016418303602</v>
       </c>
       <c r="L3">
-        <v>0.96916176826951494</v>
+        <v>0.95131356010032198</v>
       </c>
       <c r="M3">
-        <v>0.61159616378221704</v>
+        <v>0.44192284015363698</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2720,40 +2720,40 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>67.5</v>
+        <v>54.8</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>6.2</v>
+        <v>44.2</v>
       </c>
       <c r="E4">
-        <v>1.3702253440619401</v>
+        <v>1.1149808897357201</v>
       </c>
       <c r="F4">
-        <v>9.2940388488922707E-2</v>
+        <v>0.121111539193997</v>
       </c>
       <c r="G4">
-        <v>0.18785783045567001</v>
+        <v>0.89777368440771999</v>
       </c>
       <c r="H4">
-        <v>0.93019406011203898</v>
+        <v>0.91745513053611405</v>
       </c>
       <c r="I4">
-        <v>0.95392405937265901</v>
+        <v>0.927930214957709</v>
       </c>
       <c r="J4">
-        <v>0.93019406011203998</v>
+        <v>0.91745513053611405</v>
       </c>
       <c r="K4">
-        <v>0.46811426299519598</v>
+        <v>0.49842855406464998</v>
       </c>
       <c r="L4">
-        <v>1.01020632147573</v>
+        <v>1.0023376117932099</v>
       </c>
       <c r="M4">
-        <v>0.73835057254762704</v>
+        <v>0.53536901618114996</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2761,40 +2761,40 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>25.4</v>
+        <v>16.3</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>-20.5</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E5">
-        <v>0.60332796572881597</v>
+        <v>0.51045045994054095</v>
       </c>
       <c r="F5">
-        <v>0.18379400931050499</v>
+        <v>0.17523205750836901</v>
       </c>
       <c r="G5">
-        <v>0.464962126386462</v>
+        <v>0.48392300325454102</v>
       </c>
       <c r="H5">
-        <v>0.88673729685160996</v>
+        <v>0.87837110445359901</v>
       </c>
       <c r="I5">
-        <v>0.78498217394466796</v>
+        <v>0.78112016163508502</v>
       </c>
       <c r="J5">
-        <v>0.88673729685160996</v>
+        <v>0.87837110445359901</v>
       </c>
       <c r="K5">
-        <v>0.39691877484075699</v>
+        <v>0.42562866998688098</v>
       </c>
       <c r="L5">
-        <v>0.84537688322844495</v>
+        <v>0.85300644834460404</v>
       </c>
       <c r="M5">
-        <v>0.62605484990655702</v>
+        <v>0.45717365197301901</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2802,40 +2802,40 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>54.8</v>
+        <v>42.7</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>-1.8</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="E6">
-        <v>1.11282718006194</v>
+        <v>0.86734969573571996</v>
       </c>
       <c r="F6">
-        <v>0.122234561255987</v>
+        <v>0.13320633423151501</v>
       </c>
       <c r="G6">
-        <v>0.18577278069046199</v>
+        <v>0.66722904279371997</v>
       </c>
       <c r="H6">
-        <v>0.91565097784484495</v>
+        <v>0.90484792281276805</v>
       </c>
       <c r="I6">
-        <v>0.90151033916294798</v>
+        <v>0.887435831922053</v>
       </c>
       <c r="J6">
-        <v>0.91565097784484495</v>
+        <v>0.90484792281276805</v>
       </c>
       <c r="K6">
-        <v>0.46456133905040398</v>
+        <v>0.49551562091590501</v>
       </c>
       <c r="L6">
-        <v>0.96072006766502605</v>
+        <v>0.963459880417598</v>
       </c>
       <c r="M6">
-        <v>0.73274659156215105</v>
+        <v>0.53224019432428005</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2843,40 +2843,40 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>144.4</v>
+        <v>124.6</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>54.9</v>
+        <v>109.1</v>
       </c>
       <c r="E7">
-        <v>2.9305214960619401</v>
+        <v>2.5334909877357199</v>
       </c>
       <c r="F7">
-        <v>0.10041277669412101</v>
+        <v>0.123884423376002</v>
       </c>
       <c r="G7">
-        <v>1.1150556796059401</v>
+        <v>2.2184065856457198</v>
       </c>
       <c r="H7">
-        <v>0.93078577029168597</v>
+        <v>0.90777704596009101</v>
       </c>
       <c r="I7">
-        <v>0.94946093017919098</v>
+        <v>0.915820512225206</v>
       </c>
       <c r="J7">
-        <v>0.93078577029168597</v>
+        <v>0.90777704596009001</v>
       </c>
       <c r="K7">
-        <v>0.60926055216130204</v>
+        <v>0.635492805991003</v>
       </c>
       <c r="L7">
-        <v>1.0199820836896401</v>
+        <v>1.01104878110295</v>
       </c>
       <c r="M7">
-        <v>0.96097878889795396</v>
+        <v>0.68259162834694198</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2884,40 +2884,40 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>60.5</v>
+        <v>49.1</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="E8">
-        <v>1.2283358760619401</v>
+        <v>0.99736620973571999</v>
       </c>
       <c r="F8">
-        <v>0.13208980592191499</v>
+        <v>0.12726990786511999</v>
       </c>
       <c r="G8">
-        <v>0.15702122802620999</v>
+        <v>0.78827441732771997</v>
       </c>
       <c r="H8">
-        <v>0.90988591409012798</v>
+        <v>0.90067739795147606</v>
       </c>
       <c r="I8">
-        <v>0.89369366323562704</v>
+        <v>0.88465902826994103</v>
       </c>
       <c r="J8">
-        <v>0.90988591409012798</v>
+        <v>0.90067739795147606</v>
       </c>
       <c r="K8">
-        <v>0.48907248286788402</v>
+        <v>0.522304658861657</v>
       </c>
       <c r="L8">
-        <v>0.96124285380409002</v>
+        <v>0.96743697872850898</v>
       </c>
       <c r="M8">
-        <v>0.77140770168436001</v>
+        <v>0.56101467117256398</v>
       </c>
     </row>
   </sheetData>
@@ -2929,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174954FC-3560-46B8-875C-4291803A546D}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2942,65 +2942,65 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81" t="s">
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81" t="s">
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81" t="s">
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
     </row>
     <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="F2" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="82" t="s">
+      <c r="H2" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="83" t="s">
+      <c r="I2" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="82" t="s">
+      <c r="K2" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="83" t="s">
+      <c r="L2" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="84" t="s">
+      <c r="M2" s="81" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3010,19 +3010,19 @@
       </c>
       <c r="B3" s="51">
         <f>'Table 3 LEMA - raw data'!E2</f>
-        <v>0.94977537606193996</v>
+        <v>0.73191821373571997</v>
       </c>
       <c r="C3" s="52">
         <f>'Table 3 LEMA - raw data'!F2</f>
-        <v>0.340981905337637</v>
+        <v>0.346316575163579</v>
       </c>
       <c r="D3" s="53">
         <f>'Table 3 LEMA - raw data'!G2</f>
-        <v>0.29586560417854602</v>
+        <v>0.55283703019616603</v>
       </c>
       <c r="E3" s="54">
         <f>'Table 3 LEMA - raw data'!B2/100</f>
-        <v>0.46799999999999997</v>
+        <v>0.36</v>
       </c>
       <c r="F3" s="55">
         <f>'Table 3 LEMA - raw data'!C2/100</f>
@@ -3030,31 +3030,31 @@
       </c>
       <c r="G3" s="56">
         <f>'Table 3 LEMA - raw data'!D2/100</f>
-        <v>-6.9000000000000006E-2</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="H3" s="51">
         <f>'Table 3 LEMA - raw data'!K2</f>
-        <v>0.43274806461895099</v>
+        <v>0.457202436971055</v>
       </c>
       <c r="I3" s="52">
         <f>'Table 3 LEMA - raw data'!L2</f>
-        <v>0.564953094661791</v>
+        <v>0.58091958959658196</v>
       </c>
       <c r="J3" s="52">
         <f>'Table 3 LEMA - raw data'!M2</f>
-        <v>0.68256792526648402</v>
+        <v>0.49108747257900598</v>
       </c>
       <c r="K3" s="51">
         <f>'Table 3 LEMA - raw data'!H2</f>
-        <v>0.69082503808143803</v>
+        <v>0.67812486552248197</v>
       </c>
       <c r="L3" s="52">
         <f>'Table 3 LEMA - raw data'!I2</f>
-        <v>0.46154690097069101</v>
+        <v>0.47227708829139098</v>
       </c>
       <c r="M3" s="53">
         <f>'Table 3 LEMA - raw data'!J2</f>
-        <v>0.69082503808143803</v>
+        <v>0.67812486552248197</v>
       </c>
       <c r="N3" s="2"/>
     </row>
@@ -3064,19 +3064,19 @@
       </c>
       <c r="B4" s="57">
         <f>'Table 3 LEMA - raw data'!E3</f>
-        <v>2.00024414806194</v>
+        <v>1.7055407677357199</v>
       </c>
       <c r="C4" s="20">
         <f>'Table 3 LEMA - raw data'!F3</f>
-        <v>0.16927279982131699</v>
+        <v>0.182273254319129</v>
       </c>
       <c r="D4" s="21">
         <f>'Table 3 LEMA - raw data'!G3</f>
-        <v>0.52525984097393996</v>
+        <v>1.44758493082572</v>
       </c>
       <c r="E4" s="58">
         <f>'Table 3 LEMA - raw data'!B3/100</f>
-        <v>0.98499999999999999</v>
+        <v>0.83900000000000008</v>
       </c>
       <c r="F4" s="59">
         <f>'Table 3 LEMA - raw data'!C3/100</f>
@@ -3084,31 +3084,31 @@
       </c>
       <c r="G4" s="60">
         <f>'Table 3 LEMA - raw data'!D3/100</f>
-        <v>0.25900000000000001</v>
+        <v>0.71200000000000008</v>
       </c>
       <c r="H4" s="57">
         <f>'Table 3 LEMA - raw data'!K3</f>
-        <v>0.38775196783792598</v>
+        <v>0.41143016418303602</v>
       </c>
       <c r="I4" s="20">
         <f>'Table 3 LEMA - raw data'!L3</f>
-        <v>0.96916176826951494</v>
+        <v>0.95131356010032198</v>
       </c>
       <c r="J4" s="20">
         <f>'Table 3 LEMA - raw data'!M3</f>
-        <v>0.61159616378221704</v>
+        <v>0.44192284015363698</v>
       </c>
       <c r="K4" s="57">
         <f>'Table 3 LEMA - raw data'!H3</f>
-        <v>0.87769876929967305</v>
+        <v>0.86493595173328996</v>
       </c>
       <c r="L4" s="20">
         <f>'Table 3 LEMA - raw data'!I3</f>
-        <v>0.85119026125060704</v>
+        <v>0.82092275638951395</v>
       </c>
       <c r="M4" s="21">
         <f>'Table 3 LEMA - raw data'!J3</f>
-        <v>0.87769876929967305</v>
+        <v>0.86493595173328996</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -3117,19 +3117,19 @@
       </c>
       <c r="B5" s="61">
         <f>'Table 3 LEMA - raw data'!E4</f>
-        <v>1.3702253440619401</v>
+        <v>1.1149808897357201</v>
       </c>
       <c r="C5" s="73">
         <f>'Table 3 LEMA - raw data'!F4</f>
-        <v>9.2940388488922707E-2</v>
+        <v>0.121111539193997</v>
       </c>
       <c r="D5" s="14">
         <f>'Table 3 LEMA - raw data'!G4</f>
-        <v>0.18785783045567001</v>
+        <v>0.89777368440771999</v>
       </c>
       <c r="E5" s="62">
         <f>'Table 3 LEMA - raw data'!B4/100</f>
-        <v>0.67500000000000004</v>
+        <v>0.54799999999999993</v>
       </c>
       <c r="F5" s="63">
         <f>'Table 3 LEMA - raw data'!C4/100</f>
@@ -3137,31 +3137,31 @@
       </c>
       <c r="G5" s="64">
         <f>'Table 3 LEMA - raw data'!D4/100</f>
-        <v>6.2E-2</v>
+        <v>0.442</v>
       </c>
       <c r="H5" s="61">
         <f>'Table 3 LEMA - raw data'!K4</f>
-        <v>0.46811426299519598</v>
+        <v>0.49842855406464998</v>
       </c>
       <c r="I5" s="73">
         <f>'Table 3 LEMA - raw data'!L4</f>
-        <v>1.01020632147573</v>
+        <v>1.0023376117932099</v>
       </c>
       <c r="J5" s="13">
         <f>'Table 3 LEMA - raw data'!M4</f>
-        <v>0.73835057254762704</v>
+        <v>0.53536901618114996</v>
       </c>
       <c r="K5" s="72">
         <f>'Table 3 LEMA - raw data'!H4</f>
-        <v>0.93019406011203898</v>
+        <v>0.91745513053611405</v>
       </c>
       <c r="L5" s="73">
         <f>'Table 3 LEMA - raw data'!I4</f>
-        <v>0.95392405937265901</v>
+        <v>0.927930214957709</v>
       </c>
       <c r="M5" s="78">
         <f>'Table 3 LEMA - raw data'!J4</f>
-        <v>0.93019406011203998</v>
+        <v>0.91745513053611405</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -3170,19 +3170,19 @@
       </c>
       <c r="B6" s="72">
         <f>'Table 3 LEMA - raw data'!E5</f>
-        <v>0.60332796572881597</v>
+        <v>0.51045045994054095</v>
       </c>
       <c r="C6" s="20">
         <f>'Table 3 LEMA - raw data'!F5</f>
-        <v>0.18379400931050499</v>
+        <v>0.17523205750836901</v>
       </c>
       <c r="D6" s="21">
         <f>'Table 3 LEMA - raw data'!G5</f>
-        <v>0.464962126386462</v>
+        <v>0.48392300325454102</v>
       </c>
       <c r="E6" s="75">
         <f>'Table 3 LEMA - raw data'!B5/100</f>
-        <v>0.254</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="F6" s="70">
         <f>'Table 3 LEMA - raw data'!C5/100</f>
@@ -3190,31 +3190,31 @@
       </c>
       <c r="G6" s="71">
         <f>'Table 3 LEMA - raw data'!D5/100</f>
-        <v>-0.20499999999999999</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="H6" s="57">
         <f>'Table 3 LEMA - raw data'!K5</f>
-        <v>0.39691877484075699</v>
+        <v>0.42562866998688098</v>
       </c>
       <c r="I6" s="20">
         <f>'Table 3 LEMA - raw data'!L5</f>
-        <v>0.84537688322844495</v>
+        <v>0.85300644834460404</v>
       </c>
       <c r="J6" s="20">
         <f>'Table 3 LEMA - raw data'!M5</f>
-        <v>0.62605484990655702</v>
+        <v>0.45717365197301901</v>
       </c>
       <c r="K6" s="57">
         <f>'Table 3 LEMA - raw data'!H5</f>
-        <v>0.88673729685160996</v>
+        <v>0.87837110445359901</v>
       </c>
       <c r="L6" s="20">
         <f>'Table 3 LEMA - raw data'!I5</f>
-        <v>0.78498217394466796</v>
+        <v>0.78112016163508502</v>
       </c>
       <c r="M6" s="21">
         <f>'Table 3 LEMA - raw data'!J5</f>
-        <v>0.88673729685160996</v>
+        <v>0.87837110445359901</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -3223,19 +3223,19 @@
       </c>
       <c r="B7" s="61">
         <f>'Table 3 LEMA - raw data'!E6</f>
-        <v>1.11282718006194</v>
+        <v>0.86734969573571996</v>
       </c>
       <c r="C7" s="13">
         <f>'Table 3 LEMA - raw data'!F6</f>
-        <v>0.122234561255987</v>
+        <v>0.13320633423151501</v>
       </c>
       <c r="D7" s="14">
         <f>'Table 3 LEMA - raw data'!G6</f>
-        <v>0.18577278069046199</v>
+        <v>0.66722904279371997</v>
       </c>
       <c r="E7" s="62">
         <f>'Table 3 LEMA - raw data'!B6/100</f>
-        <v>0.54799999999999993</v>
+        <v>0.42700000000000005</v>
       </c>
       <c r="F7" s="63">
         <f>'Table 3 LEMA - raw data'!C6/100</f>
@@ -3243,31 +3243,31 @@
       </c>
       <c r="G7" s="76">
         <f>'Table 3 LEMA - raw data'!D6/100</f>
-        <v>-1.8000000000000002E-2</v>
+        <v>0.32799999999999996</v>
       </c>
       <c r="H7" s="61">
         <f>'Table 3 LEMA - raw data'!K6</f>
-        <v>0.46456133905040398</v>
+        <v>0.49551562091590501</v>
       </c>
       <c r="I7" s="13">
         <f>'Table 3 LEMA - raw data'!L6</f>
-        <v>0.96072006766502605</v>
+        <v>0.963459880417598</v>
       </c>
       <c r="J7" s="13">
         <f>'Table 3 LEMA - raw data'!M6</f>
-        <v>0.73274659156215105</v>
+        <v>0.53224019432428005</v>
       </c>
       <c r="K7" s="61">
         <f>'Table 3 LEMA - raw data'!H6</f>
-        <v>0.91565097784484495</v>
+        <v>0.90484792281276805</v>
       </c>
       <c r="L7" s="13">
         <f>'Table 3 LEMA - raw data'!I6</f>
-        <v>0.90151033916294798</v>
+        <v>0.887435831922053</v>
       </c>
       <c r="M7" s="14">
         <f>'Table 3 LEMA - raw data'!J6</f>
-        <v>0.91565097784484495</v>
+        <v>0.90484792281276805</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -3276,19 +3276,19 @@
       </c>
       <c r="B8" s="57">
         <f>'Table 3 LEMA - raw data'!E7</f>
-        <v>2.9305214960619401</v>
+        <v>2.5334909877357199</v>
       </c>
       <c r="C8" s="20">
         <f>'Table 3 LEMA - raw data'!F7</f>
-        <v>0.10041277669412101</v>
+        <v>0.123884423376002</v>
       </c>
       <c r="D8" s="21">
         <f>'Table 3 LEMA - raw data'!G7</f>
-        <v>1.1150556796059401</v>
+        <v>2.2184065856457198</v>
       </c>
       <c r="E8" s="69">
         <f>'Table 3 LEMA - raw data'!B7/100</f>
-        <v>1.444</v>
+        <v>1.246</v>
       </c>
       <c r="F8" s="70">
         <f>'Table 3 LEMA - raw data'!C7/100</f>
@@ -3296,31 +3296,31 @@
       </c>
       <c r="G8" s="71">
         <f>'Table 3 LEMA - raw data'!D7/100</f>
-        <v>0.54899999999999993</v>
+        <v>1.091</v>
       </c>
       <c r="H8" s="72">
         <f>'Table 3 LEMA - raw data'!K7</f>
-        <v>0.60926055216130204</v>
+        <v>0.635492805991003</v>
       </c>
       <c r="I8" s="20">
         <f>'Table 3 LEMA - raw data'!L7</f>
-        <v>1.0199820836896401</v>
+        <v>1.01104878110295</v>
       </c>
       <c r="J8" s="73">
         <f>'Table 3 LEMA - raw data'!M7</f>
-        <v>0.96097878889795396</v>
+        <v>0.68259162834694198</v>
       </c>
       <c r="K8" s="72">
         <f>'Table 3 LEMA - raw data'!H7</f>
-        <v>0.93078577029168597</v>
+        <v>0.90777704596009101</v>
       </c>
       <c r="L8" s="73">
         <f>'Table 3 LEMA - raw data'!I7</f>
-        <v>0.94946093017919098</v>
+        <v>0.915820512225206</v>
       </c>
       <c r="M8" s="78">
         <f>'Table 3 LEMA - raw data'!J7</f>
-        <v>0.93078577029168597</v>
+        <v>0.90777704596009001</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -3329,19 +3329,19 @@
       </c>
       <c r="B9" s="65">
         <f>'Table 3 LEMA - raw data'!E8</f>
-        <v>1.2283358760619401</v>
+        <v>0.99736620973571999</v>
       </c>
       <c r="C9" s="34">
         <f>'Table 3 LEMA - raw data'!F8</f>
-        <v>0.13208980592191499</v>
+        <v>0.12726990786511999</v>
       </c>
       <c r="D9" s="74">
         <f>'Table 3 LEMA - raw data'!G8</f>
-        <v>0.15702122802620999</v>
+        <v>0.78827441732771997</v>
       </c>
       <c r="E9" s="66">
         <f>'Table 3 LEMA - raw data'!B8/100</f>
-        <v>0.60499999999999998</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="F9" s="67">
         <f>'Table 3 LEMA - raw data'!C8/100</f>
@@ -3349,31 +3349,31 @@
       </c>
       <c r="G9" s="77">
         <f>'Table 3 LEMA - raw data'!D8/100</f>
-        <v>1.8000000000000002E-2</v>
+        <v>0.38799999999999996</v>
       </c>
       <c r="H9" s="65">
         <f>'Table 3 LEMA - raw data'!K8</f>
-        <v>0.48907248286788402</v>
+        <v>0.522304658861657</v>
       </c>
       <c r="I9" s="34">
         <f>'Table 3 LEMA - raw data'!L8</f>
-        <v>0.96124285380409002</v>
+        <v>0.96743697872850898</v>
       </c>
       <c r="J9" s="34">
         <f>'Table 3 LEMA - raw data'!M8</f>
-        <v>0.77140770168436001</v>
+        <v>0.56101467117256398</v>
       </c>
       <c r="K9" s="65">
         <f>'Table 3 LEMA - raw data'!H8</f>
-        <v>0.90988591409012798</v>
+        <v>0.90067739795147606</v>
       </c>
       <c r="L9" s="34">
         <f>'Table 3 LEMA - raw data'!I8</f>
-        <v>0.89369366323562704</v>
+        <v>0.88465902826994103</v>
       </c>
       <c r="M9" s="35">
         <f>'Table 3 LEMA - raw data'!J8</f>
-        <v>0.90988591409012798</v>
+        <v>0.90067739795147606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update figures and tables for revision
</commit_message>
<xml_diff>
--- a/figures+tables/Tables_FitStats_Formatted.xlsx
+++ b/figures+tables/Tables_FitStats_Formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s947z036\WorkGits\SD-6_MapWaterConservation\figures+tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133BE435-C7CF-40C8-A461-FB7F30FE0D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87242CE-D6BF-4031-936E-4BB33C55E5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 field - raw data" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="59">
   <si>
     <t>Algorithm</t>
   </si>
@@ -353,22 +353,7 @@
     <t>slope_PrecipCorrect</t>
   </si>
   <si>
-    <t>Bias_prc_AreaShift</t>
-  </si>
-  <si>
-    <t>MAE_1e7m3_AreaShift</t>
-  </si>
-  <si>
-    <t>R2_AreaShift</t>
-  </si>
-  <si>
-    <t>slope_AreaShift</t>
-  </si>
-  <si>
     <t>Precip-Adj.</t>
-  </si>
-  <si>
-    <t>Area-Adj.</t>
   </si>
   <si>
     <t>Calc.</t>
@@ -449,7 +434,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,12 +444,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,7 +593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -759,21 +738,9 @@
     <xf numFmtId="9" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -784,15 +751,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -805,43 +763,92 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1454,22 +1461,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="82" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="82" t="s">
+      <c r="E1" s="66"/>
+      <c r="F1" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="83"/>
-      <c r="H1" s="82" t="s">
+      <c r="G1" s="66"/>
+      <c r="H1" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="83"/>
+      <c r="I1" s="66"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1822,23 +1829,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="68"/>
-      <c r="B1" s="82" t="s">
+      <c r="A1" s="61"/>
+      <c r="B1" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="82" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="82" t="s">
+      <c r="E1" s="66"/>
+      <c r="F1" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="83"/>
-      <c r="H1" s="82" t="s">
+      <c r="G1" s="66"/>
+      <c r="H1" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="83"/>
+      <c r="I1" s="66"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2358,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277FF2F4-7C15-432E-B910-25206B0CD439}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I6" sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,22 +2378,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84" t="s">
+      <c r="C1" s="67"/>
+      <c r="D1" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84" t="s">
+      <c r="E1" s="67"/>
+      <c r="F1" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84" t="s">
+      <c r="G1" s="67"/>
+      <c r="H1" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="84"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2413,7 +2420,7 @@
       <c r="H2" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="97" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2449,7 +2456,7 @@
         <f>'Table 2 WRG - raw data'!C2</f>
         <v>0.71888166334803105</v>
       </c>
-      <c r="I3" s="52">
+      <c r="I3" s="53">
         <f>'Table 2 WRG - raw data'!C4</f>
         <v>0.82990617265505395</v>
       </c>
@@ -2459,7 +2466,7 @@
       <c r="A4" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="57">
+      <c r="B4" s="56">
         <f>'Table 2 WRG - raw data'!F2</f>
         <v>98.759197343525599</v>
       </c>
@@ -2467,15 +2474,15 @@
         <f>'Table 2 WRG - raw data'!F4</f>
         <v>93.808825454358299</v>
       </c>
-      <c r="D4" s="69">
+      <c r="D4" s="62">
         <f>'Table 2 WRG - raw data'!E2/100</f>
         <v>0.41899999999999998</v>
       </c>
-      <c r="E4" s="70">
+      <c r="E4" s="63">
         <f>'Table 2 WRG - raw data'!E4/100</f>
         <v>0.38400000000000001</v>
       </c>
-      <c r="F4" s="57">
+      <c r="F4" s="56">
         <f>'Table 2 WRG - raw data'!H2</f>
         <v>0.53539159921825896</v>
       </c>
@@ -2483,11 +2490,11 @@
         <f>'Table 2 WRG - raw data'!H4</f>
         <v>0.55829468693486495</v>
       </c>
-      <c r="H4" s="57">
+      <c r="H4" s="56">
         <f>'Table 2 WRG - raw data'!G2</f>
         <v>0.35484322928865197</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="21">
         <f>'Table 2 WRG - raw data'!G4</f>
         <v>0.40348024279047201</v>
       </c>
@@ -2496,7 +2503,7 @@
       <c r="A5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="61">
+      <c r="B5" s="57">
         <f>'Table 2 WRG - raw data'!B3</f>
         <v>0.86468561938909405</v>
       </c>
@@ -2504,15 +2511,15 @@
         <f>'Table 2 WRG - raw data'!B5</f>
         <v>0.66948215809220002</v>
       </c>
-      <c r="D5" s="62">
+      <c r="D5" s="58">
         <f>'Table 2 WRG - raw data'!A3/100</f>
         <v>0.57100000000000006</v>
       </c>
-      <c r="E5" s="63">
+      <c r="E5" s="59">
         <f>'Table 2 WRG - raw data'!A5/100</f>
         <v>0.41299999999999998</v>
       </c>
-      <c r="F5" s="61">
+      <c r="F5" s="57">
         <f>'Table 2 WRG - raw data'!D3</f>
         <v>0.56803530487022602</v>
       </c>
@@ -2520,48 +2527,48 @@
         <f>'Table 2 WRG - raw data'!D5</f>
         <v>0.68187133802716304</v>
       </c>
-      <c r="H5" s="61">
+      <c r="H5" s="57">
         <f>'Table 2 WRG - raw data'!C3</f>
         <v>0.79431290158147605</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="14">
         <f>'Table 2 WRG - raw data'!C5</f>
         <v>0.893584640723324</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="57">
+      <c r="B6" s="95">
         <f>'Table 2 WRG - raw data'!F3</f>
         <v>90.971653090639904</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="96">
         <f>'Table 2 WRG - raw data'!F5</f>
         <v>89.8800460460008</v>
       </c>
-      <c r="D6" s="69">
+      <c r="D6" s="80">
         <f>'Table 2 WRG - raw data'!E3/100</f>
         <v>0.41200000000000003</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="81">
         <f>'Table 2 WRG - raw data'!E5/100</f>
         <v>0.39299999999999996</v>
       </c>
-      <c r="F6" s="57">
+      <c r="F6" s="95">
         <f>'Table 2 WRG - raw data'!H3</f>
         <v>0.44300427827585298</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="96">
         <f>'Table 2 WRG - raw data'!H5</f>
         <v>0.58431264657070303</v>
       </c>
-      <c r="H6" s="57">
+      <c r="H6" s="95">
         <f>'Table 2 WRG - raw data'!G3</f>
         <v>5.2893106728812998E-2</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="98">
         <f>'Table 2 WRG - raw data'!G5</f>
         <v>0.32447301864828998</v>
       </c>
@@ -2580,10 +2587,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2592,7 +2599,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2603,37 +2610,25 @@
         <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" t="s">
         <v>56</v>
       </c>
-      <c r="M1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2644,37 +2639,25 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>26.6</v>
+        <v>0.73191821373571997</v>
       </c>
       <c r="E2">
-        <v>0.73191821373571997</v>
+        <v>0.346316575163579</v>
       </c>
       <c r="F2">
-        <v>0.346316575163579</v>
+        <v>0.67812486552248197</v>
       </c>
       <c r="G2">
-        <v>0.55283703019616603</v>
+        <v>0.47227708829139098</v>
       </c>
       <c r="H2">
-        <v>0.67812486552248197</v>
+        <v>0.457202436971055</v>
       </c>
       <c r="I2">
-        <v>0.47227708829139098</v>
-      </c>
-      <c r="J2">
-        <v>0.67812486552248197</v>
-      </c>
-      <c r="K2">
-        <v>0.457202436971055</v>
-      </c>
-      <c r="L2">
         <v>0.58091958959658196</v>
       </c>
-      <c r="M2">
-        <v>0.49108747257900598</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2685,37 +2668,25 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>71.2</v>
+        <v>1.7055407677357199</v>
       </c>
       <c r="E3">
-        <v>1.7055407677357199</v>
+        <v>0.182273254319129</v>
       </c>
       <c r="F3">
-        <v>0.182273254319129</v>
+        <v>0.86493595173328996</v>
       </c>
       <c r="G3">
-        <v>1.44758493082572</v>
+        <v>0.82092275638951395</v>
       </c>
       <c r="H3">
-        <v>0.86493595173328996</v>
+        <v>0.41143016418303602</v>
       </c>
       <c r="I3">
-        <v>0.82092275638951395</v>
-      </c>
-      <c r="J3">
-        <v>0.86493595173328996</v>
-      </c>
-      <c r="K3">
-        <v>0.41143016418303602</v>
-      </c>
-      <c r="L3">
         <v>0.95131356010032198</v>
       </c>
-      <c r="M3">
-        <v>0.44192284015363698</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2726,37 +2697,25 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>44.2</v>
+        <v>1.1149808897357201</v>
       </c>
       <c r="E4">
-        <v>1.1149808897357201</v>
+        <v>0.121111539193997</v>
       </c>
       <c r="F4">
-        <v>0.121111539193997</v>
+        <v>0.91745513053611405</v>
       </c>
       <c r="G4">
-        <v>0.89777368440771999</v>
+        <v>0.927930214957709</v>
       </c>
       <c r="H4">
-        <v>0.91745513053611405</v>
+        <v>0.49842855406464998</v>
       </c>
       <c r="I4">
-        <v>0.927930214957709</v>
-      </c>
-      <c r="J4">
-        <v>0.91745513053611405</v>
-      </c>
-      <c r="K4">
-        <v>0.49842855406464998</v>
-      </c>
-      <c r="L4">
         <v>1.0023376117932099</v>
       </c>
-      <c r="M4">
-        <v>0.53536901618114996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2767,37 +2726,25 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>8.3000000000000007</v>
+        <v>0.51045045994054095</v>
       </c>
       <c r="E5">
-        <v>0.51045045994054095</v>
+        <v>0.17523205750836901</v>
       </c>
       <c r="F5">
-        <v>0.17523205750836901</v>
+        <v>0.87837110445359901</v>
       </c>
       <c r="G5">
-        <v>0.48392300325454102</v>
+        <v>0.78112016163508502</v>
       </c>
       <c r="H5">
-        <v>0.87837110445359901</v>
+        <v>0.42562866998688098</v>
       </c>
       <c r="I5">
-        <v>0.78112016163508502</v>
-      </c>
-      <c r="J5">
-        <v>0.87837110445359901</v>
-      </c>
-      <c r="K5">
-        <v>0.42562866998688098</v>
-      </c>
-      <c r="L5">
         <v>0.85300644834460404</v>
       </c>
-      <c r="M5">
-        <v>0.45717365197301901</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2808,37 +2755,25 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>32.799999999999997</v>
+        <v>0.86734969573571996</v>
       </c>
       <c r="E6">
-        <v>0.86734969573571996</v>
+        <v>0.13320633423151501</v>
       </c>
       <c r="F6">
-        <v>0.13320633423151501</v>
+        <v>0.90484792281276805</v>
       </c>
       <c r="G6">
-        <v>0.66722904279371997</v>
+        <v>0.887435831922053</v>
       </c>
       <c r="H6">
-        <v>0.90484792281276805</v>
+        <v>0.49551562091590501</v>
       </c>
       <c r="I6">
-        <v>0.887435831922053</v>
-      </c>
-      <c r="J6">
-        <v>0.90484792281276805</v>
-      </c>
-      <c r="K6">
-        <v>0.49551562091590501</v>
-      </c>
-      <c r="L6">
         <v>0.963459880417598</v>
       </c>
-      <c r="M6">
-        <v>0.53224019432428005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2849,37 +2784,25 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>109.1</v>
+        <v>2.5334909877357199</v>
       </c>
       <c r="E7">
-        <v>2.5334909877357199</v>
+        <v>0.123884423376002</v>
       </c>
       <c r="F7">
-        <v>0.123884423376002</v>
+        <v>0.90777704596009101</v>
       </c>
       <c r="G7">
-        <v>2.2184065856457198</v>
+        <v>0.915820512225206</v>
       </c>
       <c r="H7">
-        <v>0.90777704596009101</v>
+        <v>0.635492805991003</v>
       </c>
       <c r="I7">
-        <v>0.915820512225206</v>
-      </c>
-      <c r="J7">
-        <v>0.90777704596009001</v>
-      </c>
-      <c r="K7">
-        <v>0.635492805991003</v>
-      </c>
-      <c r="L7">
         <v>1.01104878110295</v>
       </c>
-      <c r="M7">
-        <v>0.68259162834694198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2890,34 +2813,22 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>38.799999999999997</v>
+        <v>0.99736620973571999</v>
       </c>
       <c r="E8">
-        <v>0.99736620973571999</v>
+        <v>0.12726990786511999</v>
       </c>
       <c r="F8">
-        <v>0.12726990786511999</v>
+        <v>0.90067739795147606</v>
       </c>
       <c r="G8">
-        <v>0.78827441732771997</v>
+        <v>0.88465902826994103</v>
       </c>
       <c r="H8">
-        <v>0.90067739795147606</v>
+        <v>0.522304658861657</v>
       </c>
       <c r="I8">
-        <v>0.88465902826994103</v>
-      </c>
-      <c r="J8">
-        <v>0.90067739795147606</v>
-      </c>
-      <c r="K8">
-        <v>0.522304658861657</v>
-      </c>
-      <c r="L8">
         <v>0.96743697872850898</v>
-      </c>
-      <c r="M8">
-        <v>0.56101467117256398</v>
       </c>
     </row>
   </sheetData>
@@ -2927,461 +2838,334 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174954FC-3560-46B8-875C-4291803A546D}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="6.7109375" customWidth="1"/>
-    <col min="14" max="14" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="71" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="6.7109375" style="71" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="71" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="84" t="s">
+    <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="68"/>
+      <c r="B1" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84" t="s">
+      <c r="C1" s="70"/>
+      <c r="D1" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84" t="s">
+      <c r="E1" s="70"/>
+      <c r="F1" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84" t="s">
+      <c r="G1" s="70"/>
+      <c r="H1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-    </row>
-    <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="I1" s="70"/>
+    </row>
+    <row r="2" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="79" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="80" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="81" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="79" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="80" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="81" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="79" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="80" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="81" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="79" t="s">
-        <v>63</v>
-      </c>
-      <c r="L2" s="80" t="s">
-        <v>61</v>
-      </c>
-      <c r="M2" s="81" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="B2" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="85" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="87" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="87" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="87" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="51">
+      <c r="B3" s="73">
+        <f>'Table 3 LEMA - raw data'!D2</f>
+        <v>0.73191821373571997</v>
+      </c>
+      <c r="C3" s="88">
         <f>'Table 3 LEMA - raw data'!E2</f>
-        <v>0.73191821373571997</v>
-      </c>
-      <c r="C3" s="52">
-        <f>'Table 3 LEMA - raw data'!F2</f>
         <v>0.346316575163579</v>
       </c>
-      <c r="D3" s="53">
-        <f>'Table 3 LEMA - raw data'!G2</f>
-        <v>0.55283703019616603</v>
-      </c>
-      <c r="E3" s="54">
+      <c r="D3" s="75">
         <f>'Table 3 LEMA - raw data'!B2/100</f>
         <v>0.36</v>
       </c>
-      <c r="F3" s="55">
+      <c r="E3" s="91">
         <f>'Table 3 LEMA - raw data'!C2/100</f>
         <v>0</v>
       </c>
-      <c r="G3" s="56">
-        <f>'Table 3 LEMA - raw data'!D2/100</f>
-        <v>0.26600000000000001</v>
-      </c>
-      <c r="H3" s="51">
-        <f>'Table 3 LEMA - raw data'!K2</f>
+      <c r="F3" s="74">
+        <f>'Table 3 LEMA - raw data'!H2</f>
         <v>0.457202436971055</v>
       </c>
-      <c r="I3" s="52">
-        <f>'Table 3 LEMA - raw data'!L2</f>
+      <c r="G3" s="88">
+        <f>'Table 3 LEMA - raw data'!I2</f>
         <v>0.58091958959658196</v>
       </c>
-      <c r="J3" s="52">
-        <f>'Table 3 LEMA - raw data'!M2</f>
-        <v>0.49108747257900598</v>
-      </c>
-      <c r="K3" s="51">
-        <f>'Table 3 LEMA - raw data'!H2</f>
+      <c r="H3" s="74">
+        <f>'Table 3 LEMA - raw data'!F2</f>
         <v>0.67812486552248197</v>
       </c>
-      <c r="L3" s="52">
-        <f>'Table 3 LEMA - raw data'!I2</f>
+      <c r="I3" s="88">
+        <f>'Table 3 LEMA - raw data'!G2</f>
         <v>0.47227708829139098</v>
       </c>
-      <c r="M3" s="53">
-        <f>'Table 3 LEMA - raw data'!J2</f>
-        <v>0.67812486552248197</v>
-      </c>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="J3" s="76"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="93" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="57">
+        <f>'Table 3 LEMA - raw data'!D3</f>
+        <v>1.7055407677357199</v>
+      </c>
+      <c r="C4" s="14">
         <f>'Table 3 LEMA - raw data'!E3</f>
-        <v>1.7055407677357199</v>
-      </c>
-      <c r="C4" s="20">
-        <f>'Table 3 LEMA - raw data'!F3</f>
         <v>0.182273254319129</v>
       </c>
-      <c r="D4" s="21">
-        <f>'Table 3 LEMA - raw data'!G3</f>
-        <v>1.44758493082572</v>
-      </c>
-      <c r="E4" s="58">
+      <c r="D4" s="59">
         <f>'Table 3 LEMA - raw data'!B3/100</f>
         <v>0.83900000000000008</v>
       </c>
-      <c r="F4" s="59">
+      <c r="E4" s="60">
         <f>'Table 3 LEMA - raw data'!C3/100</f>
         <v>0</v>
       </c>
-      <c r="G4" s="60">
-        <f>'Table 3 LEMA - raw data'!D3/100</f>
-        <v>0.71200000000000008</v>
-      </c>
-      <c r="H4" s="57">
-        <f>'Table 3 LEMA - raw data'!K3</f>
+      <c r="F4" s="94">
+        <f>'Table 3 LEMA - raw data'!H3</f>
         <v>0.41143016418303602</v>
       </c>
-      <c r="I4" s="20">
-        <f>'Table 3 LEMA - raw data'!L3</f>
+      <c r="G4" s="14">
+        <f>'Table 3 LEMA - raw data'!I3</f>
         <v>0.95131356010032198</v>
       </c>
-      <c r="J4" s="20">
-        <f>'Table 3 LEMA - raw data'!M3</f>
-        <v>0.44192284015363698</v>
-      </c>
-      <c r="K4" s="57">
-        <f>'Table 3 LEMA - raw data'!H3</f>
+      <c r="H4" s="94">
+        <f>'Table 3 LEMA - raw data'!F3</f>
         <v>0.86493595173328996</v>
       </c>
-      <c r="L4" s="20">
-        <f>'Table 3 LEMA - raw data'!I3</f>
+      <c r="I4" s="14">
+        <f>'Table 3 LEMA - raw data'!G3</f>
         <v>0.82092275638951395</v>
       </c>
-      <c r="M4" s="21">
-        <f>'Table 3 LEMA - raw data'!J3</f>
-        <v>0.86493595173328996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="61">
+      <c r="B5" s="77">
+        <f>'Table 3 LEMA - raw data'!D4</f>
+        <v>1.1149808897357201</v>
+      </c>
+      <c r="C5" s="89">
         <f>'Table 3 LEMA - raw data'!E4</f>
-        <v>1.1149808897357201</v>
-      </c>
-      <c r="C5" s="73">
-        <f>'Table 3 LEMA - raw data'!F4</f>
         <v>0.121111539193997</v>
       </c>
-      <c r="D5" s="14">
-        <f>'Table 3 LEMA - raw data'!G4</f>
-        <v>0.89777368440771999</v>
-      </c>
-      <c r="E5" s="62">
+      <c r="D5" s="63">
         <f>'Table 3 LEMA - raw data'!B4/100</f>
         <v>0.54799999999999993</v>
       </c>
-      <c r="F5" s="63">
+      <c r="E5" s="64">
         <f>'Table 3 LEMA - raw data'!C4/100</f>
         <v>0</v>
       </c>
-      <c r="G5" s="64">
-        <f>'Table 3 LEMA - raw data'!D4/100</f>
-        <v>0.442</v>
-      </c>
-      <c r="H5" s="61">
-        <f>'Table 3 LEMA - raw data'!K4</f>
+      <c r="F5" s="86">
+        <f>'Table 3 LEMA - raw data'!H4</f>
         <v>0.49842855406464998</v>
       </c>
-      <c r="I5" s="73">
-        <f>'Table 3 LEMA - raw data'!L4</f>
+      <c r="G5" s="89">
+        <f>'Table 3 LEMA - raw data'!I4</f>
         <v>1.0023376117932099</v>
       </c>
-      <c r="J5" s="13">
-        <f>'Table 3 LEMA - raw data'!M4</f>
-        <v>0.53536901618114996</v>
-      </c>
-      <c r="K5" s="72">
-        <f>'Table 3 LEMA - raw data'!H4</f>
+      <c r="H5" s="86">
+        <f>'Table 3 LEMA - raw data'!F4</f>
         <v>0.91745513053611405</v>
       </c>
-      <c r="L5" s="73">
-        <f>'Table 3 LEMA - raw data'!I4</f>
+      <c r="I5" s="89">
+        <f>'Table 3 LEMA - raw data'!G4</f>
         <v>0.927930214957709</v>
       </c>
-      <c r="M5" s="78">
-        <f>'Table 3 LEMA - raw data'!J4</f>
-        <v>0.91745513053611405</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="72">
+      <c r="B6" s="57">
+        <f>'Table 3 LEMA - raw data'!D5</f>
+        <v>0.51045045994054095</v>
+      </c>
+      <c r="C6" s="14">
         <f>'Table 3 LEMA - raw data'!E5</f>
-        <v>0.51045045994054095</v>
-      </c>
-      <c r="C6" s="20">
-        <f>'Table 3 LEMA - raw data'!F5</f>
         <v>0.17523205750836901</v>
       </c>
-      <c r="D6" s="21">
-        <f>'Table 3 LEMA - raw data'!G5</f>
-        <v>0.48392300325454102</v>
-      </c>
-      <c r="E6" s="75">
+      <c r="D6" s="59">
         <f>'Table 3 LEMA - raw data'!B5/100</f>
         <v>0.16300000000000001</v>
       </c>
-      <c r="F6" s="70">
+      <c r="E6" s="60">
         <f>'Table 3 LEMA - raw data'!C5/100</f>
         <v>0</v>
       </c>
-      <c r="G6" s="71">
-        <f>'Table 3 LEMA - raw data'!D5/100</f>
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="H6" s="57">
-        <f>'Table 3 LEMA - raw data'!K5</f>
+      <c r="F6" s="94">
+        <f>'Table 3 LEMA - raw data'!H5</f>
         <v>0.42562866998688098</v>
       </c>
-      <c r="I6" s="20">
-        <f>'Table 3 LEMA - raw data'!L5</f>
+      <c r="G6" s="14">
+        <f>'Table 3 LEMA - raw data'!I5</f>
         <v>0.85300644834460404</v>
       </c>
-      <c r="J6" s="20">
-        <f>'Table 3 LEMA - raw data'!M5</f>
-        <v>0.45717365197301901</v>
-      </c>
-      <c r="K6" s="57">
-        <f>'Table 3 LEMA - raw data'!H5</f>
+      <c r="H6" s="94">
+        <f>'Table 3 LEMA - raw data'!F5</f>
         <v>0.87837110445359901</v>
       </c>
-      <c r="L6" s="20">
-        <f>'Table 3 LEMA - raw data'!I5</f>
+      <c r="I6" s="14">
+        <f>'Table 3 LEMA - raw data'!G5</f>
         <v>0.78112016163508502</v>
       </c>
-      <c r="M6" s="21">
-        <f>'Table 3 LEMA - raw data'!J5</f>
-        <v>0.87837110445359901</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="61">
+      <c r="B7" s="77">
+        <f>'Table 3 LEMA - raw data'!D6</f>
+        <v>0.86734969573571996</v>
+      </c>
+      <c r="C7" s="89">
         <f>'Table 3 LEMA - raw data'!E6</f>
-        <v>0.86734969573571996</v>
-      </c>
-      <c r="C7" s="13">
-        <f>'Table 3 LEMA - raw data'!F6</f>
         <v>0.13320633423151501</v>
       </c>
-      <c r="D7" s="14">
-        <f>'Table 3 LEMA - raw data'!G6</f>
-        <v>0.66722904279371997</v>
-      </c>
-      <c r="E7" s="62">
+      <c r="D7" s="63">
         <f>'Table 3 LEMA - raw data'!B6/100</f>
         <v>0.42700000000000005</v>
       </c>
-      <c r="F7" s="63">
+      <c r="E7" s="64">
         <f>'Table 3 LEMA - raw data'!C6/100</f>
         <v>0</v>
       </c>
-      <c r="G7" s="76">
-        <f>'Table 3 LEMA - raw data'!D6/100</f>
-        <v>0.32799999999999996</v>
-      </c>
-      <c r="H7" s="61">
-        <f>'Table 3 LEMA - raw data'!K6</f>
+      <c r="F7" s="86">
+        <f>'Table 3 LEMA - raw data'!H6</f>
         <v>0.49551562091590501</v>
       </c>
-      <c r="I7" s="13">
-        <f>'Table 3 LEMA - raw data'!L6</f>
+      <c r="G7" s="89">
+        <f>'Table 3 LEMA - raw data'!I6</f>
         <v>0.963459880417598</v>
       </c>
-      <c r="J7" s="13">
-        <f>'Table 3 LEMA - raw data'!M6</f>
-        <v>0.53224019432428005</v>
-      </c>
-      <c r="K7" s="61">
-        <f>'Table 3 LEMA - raw data'!H6</f>
+      <c r="H7" s="86">
+        <f>'Table 3 LEMA - raw data'!F6</f>
         <v>0.90484792281276805</v>
       </c>
-      <c r="L7" s="13">
-        <f>'Table 3 LEMA - raw data'!I6</f>
+      <c r="I7" s="89">
+        <f>'Table 3 LEMA - raw data'!G6</f>
         <v>0.887435831922053</v>
       </c>
-      <c r="M7" s="14">
-        <f>'Table 3 LEMA - raw data'!J6</f>
-        <v>0.90484792281276805</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="93" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="57">
+        <f>'Table 3 LEMA - raw data'!D7</f>
+        <v>2.5334909877357199</v>
+      </c>
+      <c r="C8" s="14">
         <f>'Table 3 LEMA - raw data'!E7</f>
-        <v>2.5334909877357199</v>
-      </c>
-      <c r="C8" s="20">
-        <f>'Table 3 LEMA - raw data'!F7</f>
         <v>0.123884423376002</v>
       </c>
-      <c r="D8" s="21">
-        <f>'Table 3 LEMA - raw data'!G7</f>
-        <v>2.2184065856457198</v>
-      </c>
-      <c r="E8" s="69">
+      <c r="D8" s="59">
         <f>'Table 3 LEMA - raw data'!B7/100</f>
         <v>1.246</v>
       </c>
-      <c r="F8" s="70">
+      <c r="E8" s="60">
         <f>'Table 3 LEMA - raw data'!C7/100</f>
         <v>0</v>
       </c>
-      <c r="G8" s="71">
-        <f>'Table 3 LEMA - raw data'!D7/100</f>
-        <v>1.091</v>
-      </c>
-      <c r="H8" s="72">
-        <f>'Table 3 LEMA - raw data'!K7</f>
+      <c r="F8" s="94">
+        <f>'Table 3 LEMA - raw data'!H7</f>
         <v>0.635492805991003</v>
       </c>
-      <c r="I8" s="20">
-        <f>'Table 3 LEMA - raw data'!L7</f>
+      <c r="G8" s="14">
+        <f>'Table 3 LEMA - raw data'!I7</f>
         <v>1.01104878110295</v>
       </c>
-      <c r="J8" s="73">
-        <f>'Table 3 LEMA - raw data'!M7</f>
-        <v>0.68259162834694198</v>
-      </c>
-      <c r="K8" s="72">
-        <f>'Table 3 LEMA - raw data'!H7</f>
+      <c r="H8" s="94">
+        <f>'Table 3 LEMA - raw data'!F7</f>
         <v>0.90777704596009101</v>
       </c>
-      <c r="L8" s="73">
-        <f>'Table 3 LEMA - raw data'!I7</f>
+      <c r="I8" s="14">
+        <f>'Table 3 LEMA - raw data'!G7</f>
         <v>0.915820512225206</v>
       </c>
-      <c r="M8" s="78">
-        <f>'Table 3 LEMA - raw data'!J7</f>
-        <v>0.90777704596009001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="65">
+      <c r="B9" s="78">
+        <f>'Table 3 LEMA - raw data'!D8</f>
+        <v>0.99736620973571999</v>
+      </c>
+      <c r="C9" s="90">
         <f>'Table 3 LEMA - raw data'!E8</f>
-        <v>0.99736620973571999</v>
-      </c>
-      <c r="C9" s="34">
-        <f>'Table 3 LEMA - raw data'!F8</f>
         <v>0.12726990786511999</v>
       </c>
-      <c r="D9" s="74">
-        <f>'Table 3 LEMA - raw data'!G8</f>
-        <v>0.78827441732771997</v>
-      </c>
-      <c r="E9" s="66">
+      <c r="D9" s="81">
         <f>'Table 3 LEMA - raw data'!B8/100</f>
         <v>0.49099999999999999</v>
       </c>
-      <c r="F9" s="67">
+      <c r="E9" s="92">
         <f>'Table 3 LEMA - raw data'!C8/100</f>
         <v>0</v>
       </c>
-      <c r="G9" s="77">
-        <f>'Table 3 LEMA - raw data'!D8/100</f>
-        <v>0.38799999999999996</v>
-      </c>
-      <c r="H9" s="65">
-        <f>'Table 3 LEMA - raw data'!K8</f>
+      <c r="F9" s="79">
+        <f>'Table 3 LEMA - raw data'!H8</f>
         <v>0.522304658861657</v>
       </c>
-      <c r="I9" s="34">
-        <f>'Table 3 LEMA - raw data'!L8</f>
+      <c r="G9" s="90">
+        <f>'Table 3 LEMA - raw data'!I8</f>
         <v>0.96743697872850898</v>
       </c>
-      <c r="J9" s="34">
-        <f>'Table 3 LEMA - raw data'!M8</f>
-        <v>0.56101467117256398</v>
-      </c>
-      <c r="K9" s="65">
-        <f>'Table 3 LEMA - raw data'!H8</f>
+      <c r="H9" s="79">
+        <f>'Table 3 LEMA - raw data'!F8</f>
         <v>0.90067739795147606</v>
       </c>
-      <c r="L9" s="34">
-        <f>'Table 3 LEMA - raw data'!I8</f>
+      <c r="I9" s="90">
+        <f>'Table 3 LEMA - raw data'!G8</f>
         <v>0.88465902826994103</v>
-      </c>
-      <c r="M9" s="35">
-        <f>'Table 3 LEMA - raw data'!J8</f>
-        <v>0.90067739795147606</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tweaks to Fig 5 and 7
</commit_message>
<xml_diff>
--- a/figures+tables/Tables_FitStats_Formatted.xlsx
+++ b/figures+tables/Tables_FitStats_Formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s947z036\WorkGits\SD-6_MapWaterConservation\figures+tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87242CE-D6BF-4031-936E-4BB33C55E5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7BC8DB-D1CC-4AB1-AA77-6B9339E4FC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18120" yWindow="-5925" windowWidth="18240" windowHeight="28440" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 field - raw data" sheetId="5" r:id="rId1"/>
@@ -593,7 +593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -763,41 +763,19 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -806,27 +784,20 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,20 +806,23 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1461,22 +1435,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="65" t="s">
+      <c r="C1" s="83"/>
+      <c r="D1" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="65" t="s">
+      <c r="E1" s="83"/>
+      <c r="F1" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="65" t="s">
+      <c r="G1" s="83"/>
+      <c r="H1" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="66"/>
+      <c r="I1" s="83"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1830,22 +1804,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="61"/>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="65" t="s">
+      <c r="C1" s="83"/>
+      <c r="D1" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="65" t="s">
+      <c r="E1" s="83"/>
+      <c r="F1" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="65" t="s">
+      <c r="G1" s="83"/>
+      <c r="H1" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="66"/>
+      <c r="I1" s="83"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2187,7 +2161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BDAD93-B6AB-4202-9CA1-EDDEC2C0863F}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:J5"/>
     </sheetView>
   </sheetViews>
@@ -2366,7 +2340,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I6" sqref="A1:I6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2378,22 +2352,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67" t="s">
+      <c r="C1" s="84"/>
+      <c r="D1" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67" t="s">
+      <c r="E1" s="84"/>
+      <c r="F1" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67" t="s">
+      <c r="G1" s="84"/>
+      <c r="H1" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="67"/>
+      <c r="I1" s="84"/>
     </row>
     <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2420,7 +2394,7 @@
       <c r="H2" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="97" t="s">
+      <c r="I2" s="81" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2540,35 +2514,35 @@
       <c r="A6" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="95">
+      <c r="B6" s="68">
         <f>'Table 2 WRG - raw data'!F3</f>
         <v>90.971653090639904</v>
       </c>
-      <c r="C6" s="96">
+      <c r="C6" s="69">
         <f>'Table 2 WRG - raw data'!F5</f>
         <v>89.8800460460008</v>
       </c>
-      <c r="D6" s="80">
+      <c r="D6" s="70">
         <f>'Table 2 WRG - raw data'!E3/100</f>
         <v>0.41200000000000003</v>
       </c>
-      <c r="E6" s="81">
+      <c r="E6" s="71">
         <f>'Table 2 WRG - raw data'!E5/100</f>
         <v>0.39299999999999996</v>
       </c>
-      <c r="F6" s="95">
+      <c r="F6" s="68">
         <f>'Table 2 WRG - raw data'!H3</f>
         <v>0.44300427827585298</v>
       </c>
-      <c r="G6" s="96">
+      <c r="G6" s="69">
         <f>'Table 2 WRG - raw data'!H5</f>
         <v>0.58431264657070303</v>
       </c>
-      <c r="H6" s="95">
+      <c r="H6" s="68">
         <f>'Table 2 WRG - raw data'!G3</f>
         <v>5.2893106728812998E-2</v>
       </c>
-      <c r="I6" s="98">
+      <c r="I6" s="77">
         <f>'Table 2 WRG - raw data'!G5</f>
         <v>0.32447301864828998</v>
       </c>
@@ -2840,106 +2814,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174954FC-3560-46B8-875C-4291803A546D}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="71" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="6.7109375" style="71" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="71" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="71"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="6.7109375" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="68"/>
-      <c r="B1" s="69" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="69" t="s">
+      <c r="C1" s="86"/>
+      <c r="D1" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="70"/>
-      <c r="F1" s="69" t="s">
+      <c r="E1" s="86"/>
+      <c r="F1" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="70"/>
-      <c r="H1" s="69" t="s">
+      <c r="G1" s="86"/>
+      <c r="H1" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="70"/>
+      <c r="I1" s="86"/>
     </row>
     <row r="2" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="87" t="s">
+      <c r="E2" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="87" t="s">
+      <c r="G2" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="87" t="s">
+      <c r="I2" s="75" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="73">
+      <c r="B3" s="65">
         <f>'Table 3 LEMA - raw data'!D2</f>
         <v>0.73191821373571997</v>
       </c>
-      <c r="C3" s="88">
+      <c r="C3" s="76">
         <f>'Table 3 LEMA - raw data'!E2</f>
         <v>0.346316575163579</v>
       </c>
-      <c r="D3" s="75">
+      <c r="D3" s="67">
         <f>'Table 3 LEMA - raw data'!B2/100</f>
         <v>0.36</v>
       </c>
-      <c r="E3" s="91">
+      <c r="E3" s="78">
         <f>'Table 3 LEMA - raw data'!C2/100</f>
         <v>0</v>
       </c>
-      <c r="F3" s="74">
+      <c r="F3" s="66">
         <f>'Table 3 LEMA - raw data'!H2</f>
         <v>0.457202436971055</v>
       </c>
-      <c r="G3" s="88">
+      <c r="G3" s="76">
         <f>'Table 3 LEMA - raw data'!I2</f>
         <v>0.58091958959658196</v>
       </c>
-      <c r="H3" s="74">
+      <c r="H3" s="66">
         <f>'Table 3 LEMA - raw data'!F2</f>
         <v>0.67812486552248197</v>
       </c>
-      <c r="I3" s="88">
+      <c r="I3" s="76">
         <f>'Table 3 LEMA - raw data'!G2</f>
         <v>0.47227708829139098</v>
       </c>
-      <c r="J3" s="76"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="80" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="57">
@@ -2958,7 +2931,7 @@
         <f>'Table 3 LEMA - raw data'!C3/100</f>
         <v>0</v>
       </c>
-      <c r="F4" s="94">
+      <c r="F4" s="13">
         <f>'Table 3 LEMA - raw data'!H3</f>
         <v>0.41143016418303602</v>
       </c>
@@ -2966,7 +2939,7 @@
         <f>'Table 3 LEMA - raw data'!I3</f>
         <v>0.95131356010032198</v>
       </c>
-      <c r="H4" s="94">
+      <c r="H4" s="13">
         <f>'Table 3 LEMA - raw data'!F3</f>
         <v>0.86493595173328996</v>
       </c>
@@ -2976,14 +2949,14 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="77">
+      <c r="B5" s="56">
         <f>'Table 3 LEMA - raw data'!D4</f>
         <v>1.1149808897357201</v>
       </c>
-      <c r="C5" s="89">
+      <c r="C5" s="21">
         <f>'Table 3 LEMA - raw data'!E4</f>
         <v>0.121111539193997</v>
       </c>
@@ -2995,25 +2968,25 @@
         <f>'Table 3 LEMA - raw data'!C4/100</f>
         <v>0</v>
       </c>
-      <c r="F5" s="86">
+      <c r="F5" s="20">
         <f>'Table 3 LEMA - raw data'!H4</f>
         <v>0.49842855406464998</v>
       </c>
-      <c r="G5" s="89">
+      <c r="G5" s="21">
         <f>'Table 3 LEMA - raw data'!I4</f>
         <v>1.0023376117932099</v>
       </c>
-      <c r="H5" s="86">
+      <c r="H5" s="20">
         <f>'Table 3 LEMA - raw data'!F4</f>
         <v>0.91745513053611405</v>
       </c>
-      <c r="I5" s="89">
+      <c r="I5" s="21">
         <f>'Table 3 LEMA - raw data'!G4</f>
         <v>0.927930214957709</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="80" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="57">
@@ -3032,7 +3005,7 @@
         <f>'Table 3 LEMA - raw data'!C5/100</f>
         <v>0</v>
       </c>
-      <c r="F6" s="94">
+      <c r="F6" s="13">
         <f>'Table 3 LEMA - raw data'!H5</f>
         <v>0.42562866998688098</v>
       </c>
@@ -3040,7 +3013,7 @@
         <f>'Table 3 LEMA - raw data'!I5</f>
         <v>0.85300644834460404</v>
       </c>
-      <c r="H6" s="94">
+      <c r="H6" s="13">
         <f>'Table 3 LEMA - raw data'!F5</f>
         <v>0.87837110445359901</v>
       </c>
@@ -3050,14 +3023,14 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="77">
+      <c r="B7" s="56">
         <f>'Table 3 LEMA - raw data'!D6</f>
         <v>0.86734969573571996</v>
       </c>
-      <c r="C7" s="89">
+      <c r="C7" s="21">
         <f>'Table 3 LEMA - raw data'!E6</f>
         <v>0.13320633423151501</v>
       </c>
@@ -3069,25 +3042,25 @@
         <f>'Table 3 LEMA - raw data'!C6/100</f>
         <v>0</v>
       </c>
-      <c r="F7" s="86">
+      <c r="F7" s="20">
         <f>'Table 3 LEMA - raw data'!H6</f>
         <v>0.49551562091590501</v>
       </c>
-      <c r="G7" s="89">
+      <c r="G7" s="21">
         <f>'Table 3 LEMA - raw data'!I6</f>
         <v>0.963459880417598</v>
       </c>
-      <c r="H7" s="86">
+      <c r="H7" s="20">
         <f>'Table 3 LEMA - raw data'!F6</f>
         <v>0.90484792281276805</v>
       </c>
-      <c r="I7" s="89">
+      <c r="I7" s="21">
         <f>'Table 3 LEMA - raw data'!G6</f>
         <v>0.887435831922053</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="80" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="57">
@@ -3106,7 +3079,7 @@
         <f>'Table 3 LEMA - raw data'!C7/100</f>
         <v>0</v>
       </c>
-      <c r="F8" s="94">
+      <c r="F8" s="13">
         <f>'Table 3 LEMA - raw data'!H7</f>
         <v>0.635492805991003</v>
       </c>
@@ -3114,7 +3087,7 @@
         <f>'Table 3 LEMA - raw data'!I7</f>
         <v>1.01104878110295</v>
       </c>
-      <c r="H8" s="94">
+      <c r="H8" s="13">
         <f>'Table 3 LEMA - raw data'!F7</f>
         <v>0.90777704596009101</v>
       </c>
@@ -3124,38 +3097,38 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="83" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="78">
+      <c r="B9" s="68">
         <f>'Table 3 LEMA - raw data'!D8</f>
         <v>0.99736620973571999</v>
       </c>
-      <c r="C9" s="90">
+      <c r="C9" s="77">
         <f>'Table 3 LEMA - raw data'!E8</f>
         <v>0.12726990786511999</v>
       </c>
-      <c r="D9" s="81">
+      <c r="D9" s="71">
         <f>'Table 3 LEMA - raw data'!B8/100</f>
         <v>0.49099999999999999</v>
       </c>
-      <c r="E9" s="92">
+      <c r="E9" s="79">
         <f>'Table 3 LEMA - raw data'!C8/100</f>
         <v>0</v>
       </c>
-      <c r="F9" s="79">
+      <c r="F9" s="69">
         <f>'Table 3 LEMA - raw data'!H8</f>
         <v>0.522304658861657</v>
       </c>
-      <c r="G9" s="90">
+      <c r="G9" s="77">
         <f>'Table 3 LEMA - raw data'!I8</f>
         <v>0.96743697872850898</v>
       </c>
-      <c r="H9" s="79">
+      <c r="H9" s="69">
         <f>'Table 3 LEMA - raw data'!F8</f>
         <v>0.90067739795147606</v>
       </c>
-      <c r="I9" s="90">
+      <c r="I9" s="77">
         <f>'Table 3 LEMA - raw data'!G8</f>
         <v>0.88465902826994103</v>
       </c>

</xml_diff>